<commit_message>
cambio de nombres de columnas
</commit_message>
<xml_diff>
--- a/resumen_localidades.xlsx
+++ b/resumen_localidades.xlsx
@@ -467,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A6:K63"/>
+  <dimension ref="A6:K67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -639,32 +639,32 @@
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
-          <t>Gobernador Costa</t>
+          <t>El Maiten</t>
         </is>
       </c>
       <c r="D9" s="5" t="n">
-        <v>45789.62898148148</v>
+        <v>45924.47306712963</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>45789.67918981481</v>
+        <v>45924.54931712963</v>
       </c>
       <c r="F9" s="4" t="n">
-        <v>759</v>
+        <v>1042</v>
       </c>
       <c r="G9" s="4" t="inlineStr">
         <is>
-          <t>01:12:18</t>
+          <t>01:44:00</t>
         </is>
       </c>
       <c r="H9" s="4" t="n">
-        <v>2.899</v>
+        <v>2.321</v>
       </c>
       <c r="I9" s="4" t="n">
-        <v>1.11344639852293</v>
+        <v>0.7137122732006727</v>
       </c>
       <c r="J9" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-51927249-APN- - SDYME#ENACOM</t>
+          <t>EX-2025-107280605- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K9" s="4" t="inlineStr">
@@ -686,32 +686,32 @@
       </c>
       <c r="C10" s="4" t="inlineStr">
         <is>
-          <t>Jose de San Martín</t>
+          <t>Gobernador Costa</t>
         </is>
       </c>
       <c r="D10" s="5" t="n">
-        <v>45790.40565972222</v>
+        <v>45789.62898148148</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>45790.45607638889</v>
+        <v>45789.67918981481</v>
       </c>
       <c r="F10" s="4" t="n">
-        <v>770</v>
+        <v>759</v>
       </c>
       <c r="G10" s="4" t="inlineStr">
         <is>
-          <t>01:12:36</t>
+          <t>01:12:18</t>
         </is>
       </c>
       <c r="H10" s="4" t="n">
-        <v>1.863</v>
+        <v>2.899</v>
       </c>
       <c r="I10" s="4" t="n">
-        <v>0.4598313680449851</v>
+        <v>1.11344639852293</v>
       </c>
       <c r="J10" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-51925383-APN- - SDYME#ENACOM</t>
+          <t>EX-2025-51927249-APN- - SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K10" s="4" t="inlineStr">
@@ -733,32 +733,32 @@
       </c>
       <c r="C11" s="4" t="inlineStr">
         <is>
-          <t>Rada Tilly</t>
+          <t>Jose de San Martín</t>
         </is>
       </c>
       <c r="D11" s="5" t="n">
-        <v>45786.41888888889</v>
+        <v>45790.40565972222</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>45805.66069444444</v>
+        <v>45790.45607638889</v>
       </c>
       <c r="F11" s="4" t="n">
-        <v>2878</v>
+        <v>770</v>
       </c>
       <c r="G11" s="4" t="inlineStr">
         <is>
-          <t>06:51:55</t>
+          <t>01:12:36</t>
         </is>
       </c>
       <c r="H11" s="4" t="n">
-        <v>3.21</v>
+        <v>1.863</v>
       </c>
       <c r="I11" s="4" t="n">
-        <v>1.365158095935607</v>
+        <v>0.4598313680449851</v>
       </c>
       <c r="J11" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-57494683-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-51925383-APN- - SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K11" s="4" t="inlineStr">
@@ -780,37 +780,37 @@
       </c>
       <c r="C12" s="4" t="inlineStr">
         <is>
-          <t>Río Mayo</t>
+          <t>Puerto Madryn</t>
         </is>
       </c>
       <c r="D12" s="5" t="n">
-        <v>45791.45833333334</v>
+        <v>45817.59449074074</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>45791.50844907408</v>
+        <v>45821.42857638889</v>
       </c>
       <c r="F12" s="4" t="n">
-        <v>852</v>
+        <v>10175</v>
       </c>
       <c r="G12" s="4" t="inlineStr">
         <is>
-          <t>01:12:10</t>
+          <t>17:03:07</t>
         </is>
       </c>
       <c r="H12" s="4" t="n">
-        <v>8.367000000000001</v>
+        <v>10.744</v>
       </c>
       <c r="I12" s="4" t="n">
-        <v>9.27496804747588</v>
+        <v>15.29342943225263</v>
       </c>
       <c r="J12" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-51927482-APN- - SDYME#ENACOM</t>
+          <t>EX-2025-65041629-APN- - SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K12" s="4" t="inlineStr">
         <is>
-          <t>EF0391</t>
+          <t>EF1891</t>
         </is>
       </c>
     </row>
@@ -827,32 +827,32 @@
       </c>
       <c r="C13" s="4" t="inlineStr">
         <is>
-          <t>Río Pico</t>
+          <t>Rada Tilly</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>45790.61751157408</v>
+        <v>45786.41888888889</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>45790.66715277778</v>
+        <v>45805.66069444444</v>
       </c>
       <c r="F13" s="4" t="n">
-        <v>684</v>
+        <v>2878</v>
       </c>
       <c r="G13" s="4" t="inlineStr">
         <is>
-          <t>01:11:29</t>
+          <t>06:51:55</t>
         </is>
       </c>
       <c r="H13" s="4" t="n">
-        <v>1.843</v>
+        <v>3.21</v>
       </c>
       <c r="I13" s="4" t="n">
-        <v>0.4500114402423874</v>
+        <v>1.365158095935607</v>
       </c>
       <c r="J13" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-51931624-APN- - SDYME#ENACOM</t>
+          <t>EX-2025-57494683-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K13" s="4" t="inlineStr">
@@ -874,37 +874,37 @@
       </c>
       <c r="C14" s="4" t="inlineStr">
         <is>
-          <t>Sarmiento</t>
+          <t>Rawson</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>45791.65675925926</v>
+        <v>45852.5327662037</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>45792.49758101852</v>
+        <v>45854.55157407407</v>
       </c>
       <c r="F14" s="4" t="n">
-        <v>2499</v>
+        <v>5438</v>
       </c>
       <c r="G14" s="4" t="inlineStr">
         <is>
-          <t>04:10:03</t>
+          <t>08:22:28</t>
         </is>
       </c>
       <c r="H14" s="4" t="n">
-        <v>5.587</v>
+        <v>10.067</v>
       </c>
       <c r="I14" s="4" t="n">
-        <v>4.135520965585604</v>
+        <v>13.42681550419805</v>
       </c>
       <c r="J14" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-51931433-APN- - SDYME#ENACOM</t>
+          <t>EX-2025- 78894383- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K14" s="4" t="inlineStr">
         <is>
-          <t>EF0391</t>
+          <t>EF1891</t>
         </is>
       </c>
     </row>
@@ -916,37 +916,37 @@
       </c>
       <c r="B15" s="4" t="inlineStr">
         <is>
-          <t>Santa Cruz</t>
+          <t>Chubut</t>
         </is>
       </c>
       <c r="C15" s="4" t="inlineStr">
         <is>
-          <t>28 de Noviembre</t>
+          <t>Río Mayo</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>45722.52990740741</v>
+        <v>45791.45833333334</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>45722.77141203704</v>
+        <v>45791.50844907408</v>
       </c>
       <c r="F15" s="4" t="n">
-        <v>1328</v>
+        <v>852</v>
       </c>
       <c r="G15" s="4" t="inlineStr">
         <is>
-          <t>03:12:59</t>
+          <t>01:12:10</t>
         </is>
       </c>
       <c r="H15" s="4" t="n">
-        <v>3.459</v>
+        <v>8.367000000000001</v>
       </c>
       <c r="I15" s="4" t="n">
-        <v>1.585163297370652</v>
+        <v>9.27496804747588</v>
       </c>
       <c r="J15" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-26350283- -APNSDYME# ENACOM</t>
+          <t>EX-2025-51927482-APN- - SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K15" s="4" t="inlineStr">
@@ -963,37 +963,37 @@
       </c>
       <c r="B16" s="4" t="inlineStr">
         <is>
-          <t>Santa Cruz</t>
+          <t>Chubut</t>
         </is>
       </c>
       <c r="C16" s="4" t="inlineStr">
         <is>
-          <t>Cañadon Seco</t>
+          <t>Río Pico</t>
         </is>
       </c>
       <c r="D16" s="5" t="n">
-        <v>45772.44009259259</v>
+        <v>45790.61751157408</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>45772.48277777778</v>
+        <v>45790.66715277778</v>
       </c>
       <c r="F16" s="4" t="n">
-        <v>566</v>
+        <v>684</v>
       </c>
       <c r="G16" s="4" t="inlineStr">
         <is>
-          <t>01:01:28</t>
+          <t>01:11:29</t>
         </is>
       </c>
       <c r="H16" s="4" t="n">
-        <v>0.848</v>
+        <v>1.843</v>
       </c>
       <c r="I16" s="4" t="n">
-        <v>0.09527184784888333</v>
+        <v>0.4500114402423874</v>
       </c>
       <c r="J16" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-44885465- -APNSDYME# ENACOM</t>
+          <t>EX-2025-51931624-APN- - SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K16" s="4" t="inlineStr">
@@ -1010,37 +1010,37 @@
       </c>
       <c r="B17" s="4" t="inlineStr">
         <is>
-          <t>Santa Cruz</t>
+          <t>Chubut</t>
         </is>
       </c>
       <c r="C17" s="4" t="inlineStr">
         <is>
-          <t>El Calafate</t>
+          <t>Sarmiento</t>
         </is>
       </c>
       <c r="D17" s="5" t="n">
-        <v>45725.38012731481</v>
+        <v>45791.65675925926</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>45725.89113425926</v>
+        <v>45792.49758101852</v>
       </c>
       <c r="F17" s="4" t="n">
-        <v>5098</v>
+        <v>2499</v>
       </c>
       <c r="G17" s="4" t="inlineStr">
         <is>
-          <t>08:31:23</t>
+          <t>04:10:03</t>
         </is>
       </c>
       <c r="H17" s="4" t="n">
-        <v>5.991</v>
+        <v>5.587</v>
       </c>
       <c r="I17" s="4" t="n">
-        <v>4.755229952846593</v>
+        <v>4.135520965585604</v>
       </c>
       <c r="J17" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-26350807- -APNSDYME# ENACOM</t>
+          <t>EX-2025-51931433-APN- - SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K17" s="4" t="inlineStr">
@@ -1057,42 +1057,42 @@
       </c>
       <c r="B18" s="4" t="inlineStr">
         <is>
-          <t>Santa Cruz</t>
+          <t>Chubut</t>
         </is>
       </c>
       <c r="C18" s="4" t="inlineStr">
         <is>
-          <t>El Chalten</t>
+          <t>Trelew</t>
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>45724.53105324074</v>
+        <v>45854.63928240741</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>45724.5831712963</v>
+        <v>45856.53826388889</v>
       </c>
       <c r="F18" s="4" t="n">
-        <v>458</v>
+        <v>8067</v>
       </c>
       <c r="G18" s="4" t="inlineStr">
         <is>
-          <t>01:15:03</t>
+          <t>12:46:48</t>
         </is>
       </c>
       <c r="H18" s="4" t="n">
-        <v>5.076</v>
+        <v>10.925</v>
       </c>
       <c r="I18" s="4" t="n">
-        <v>3.413627362357058</v>
+        <v>15.81305478054409</v>
       </c>
       <c r="J18" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-26350683- -APNSDYME# ENACOM</t>
+          <t>EX- 2025-78894044- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K18" s="4" t="inlineStr">
         <is>
-          <t>EF0391</t>
+          <t>EF1891</t>
         </is>
       </c>
     </row>
@@ -1109,32 +1109,32 @@
       </c>
       <c r="C19" s="4" t="inlineStr">
         <is>
-          <t>Fitz Roy</t>
+          <t>28 de Noviembre</t>
         </is>
       </c>
       <c r="D19" s="5" t="n">
-        <v>45777.47289351852</v>
+        <v>45722.52990740741</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>45777.50890046296</v>
+        <v>45722.77141203704</v>
       </c>
       <c r="F19" s="4" t="n">
-        <v>442</v>
+        <v>1328</v>
       </c>
       <c r="G19" s="4" t="inlineStr">
         <is>
-          <t>00:51:51</t>
+          <t>03:12:59</t>
         </is>
       </c>
       <c r="H19" s="4" t="n">
-        <v>1.221</v>
+        <v>3.459</v>
       </c>
       <c r="I19" s="4" t="n">
-        <v>0.1975168778353022</v>
+        <v>1.585163297370652</v>
       </c>
       <c r="J19" s="4" t="inlineStr">
         <is>
-          <t>EX-2025- 46399573- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-26350283- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K19" s="4" t="inlineStr">
@@ -1156,32 +1156,32 @@
       </c>
       <c r="C20" s="4" t="inlineStr">
         <is>
-          <t>Jaramillo</t>
+          <t>Cañadon Seco</t>
         </is>
       </c>
       <c r="D20" s="5" t="n">
-        <v>45775.47744212963</v>
+        <v>45772.44009259259</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>45775.49759259259</v>
+        <v>45772.48277777778</v>
       </c>
       <c r="F20" s="4" t="n">
-        <v>301</v>
+        <v>566</v>
       </c>
       <c r="G20" s="4" t="inlineStr">
         <is>
-          <t>00:29:01</t>
+          <t>01:01:28</t>
         </is>
       </c>
       <c r="H20" s="4" t="n">
-        <v>1.759</v>
+        <v>0.848</v>
       </c>
       <c r="I20" s="4" t="n">
-        <v>0.4099251488854474</v>
+        <v>0.09527184784888333</v>
       </c>
       <c r="J20" s="4" t="inlineStr">
         <is>
-          <t>EX-2025- 46399813- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-44885465- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K20" s="4" t="inlineStr">
@@ -1203,32 +1203,32 @@
       </c>
       <c r="C21" s="4" t="inlineStr">
         <is>
-          <t>Koluel Kayke</t>
+          <t>El Calafate</t>
         </is>
       </c>
       <c r="D21" s="5" t="n">
-        <v>45770.76137731481</v>
+        <v>45725.38012731481</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>45770.7769212963</v>
+        <v>45725.89113425926</v>
       </c>
       <c r="F21" s="4" t="n">
-        <v>224</v>
+        <v>5098</v>
       </c>
       <c r="G21" s="4" t="inlineStr">
         <is>
-          <t>00:22:23</t>
+          <t>08:31:23</t>
         </is>
       </c>
       <c r="H21" s="4" t="n">
-        <v>1.528</v>
+        <v>5.991</v>
       </c>
       <c r="I21" s="4" t="n">
-        <v>0.3093282557293622</v>
+        <v>4.755229952846593</v>
       </c>
       <c r="J21" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-44888593- -APNSDYME# ENACOM</t>
+          <t>EX-2025-26350807- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K21" s="4" t="inlineStr">
@@ -1250,32 +1250,32 @@
       </c>
       <c r="C22" s="4" t="inlineStr">
         <is>
-          <t>Las Heras</t>
+          <t>El Chalten</t>
         </is>
       </c>
       <c r="D22" s="5" t="n">
-        <v>45769.6825925926</v>
+        <v>45724.53105324074</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>45770.69950231481</v>
+        <v>45724.5831712963</v>
       </c>
       <c r="F22" s="4" t="n">
-        <v>3469</v>
+        <v>458</v>
       </c>
       <c r="G22" s="4" t="inlineStr">
         <is>
-          <t>06:13:06</t>
+          <t>01:15:03</t>
         </is>
       </c>
       <c r="H22" s="4" t="n">
-        <v>4.318</v>
+        <v>5.076</v>
       </c>
       <c r="I22" s="4" t="n">
-        <v>2.470234370621722</v>
+        <v>3.413627362357058</v>
       </c>
       <c r="J22" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-44888902- -APNSDYME# ENACOM</t>
+          <t>EX-2025-26350683- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K22" s="4" t="inlineStr">
@@ -1297,32 +1297,32 @@
       </c>
       <c r="C23" s="4" t="inlineStr">
         <is>
-          <t>Los Antiguos</t>
+          <t>Fitz Roy</t>
         </is>
       </c>
       <c r="D23" s="5" t="n">
-        <v>45769.42946759259</v>
+        <v>45777.47289351852</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>45769.51760416666</v>
+        <v>45777.50890046296</v>
       </c>
       <c r="F23" s="4" t="n">
-        <v>1085</v>
+        <v>442</v>
       </c>
       <c r="G23" s="4" t="inlineStr">
         <is>
-          <t>02:02:41</t>
+          <t>00:51:51</t>
         </is>
       </c>
       <c r="H23" s="4" t="n">
-        <v>2.739</v>
+        <v>1.221</v>
       </c>
       <c r="I23" s="4" t="n">
-        <v>0.9939326306847305</v>
+        <v>0.1975168778353022</v>
       </c>
       <c r="J23" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-44890916- -APNSDYME# ENACOM</t>
+          <t>EX-2025- 46399573- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K23" s="4" t="inlineStr">
@@ -1344,32 +1344,32 @@
       </c>
       <c r="C24" s="4" t="inlineStr">
         <is>
-          <t>Perito Moreno</t>
+          <t>Jaramillo</t>
         </is>
       </c>
       <c r="D24" s="5" t="n">
-        <v>45768.63813657407</v>
+        <v>45775.47744212963</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>45768.7884837963</v>
+        <v>45775.49759259259</v>
       </c>
       <c r="F24" s="4" t="n">
-        <v>1350</v>
+        <v>301</v>
       </c>
       <c r="G24" s="4" t="inlineStr">
         <is>
-          <t>02:53:22</t>
+          <t>00:29:01</t>
         </is>
       </c>
       <c r="H24" s="4" t="n">
-        <v>11.549</v>
+        <v>1.759</v>
       </c>
       <c r="I24" s="4" t="n">
-        <v>17.67102115722788</v>
+        <v>0.4099251488854474</v>
       </c>
       <c r="J24" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-44890944- -APNSDYME# ENACOM</t>
+          <t>EX-2025- 46399813- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K24" s="4" t="inlineStr">
@@ -1391,32 +1391,32 @@
       </c>
       <c r="C25" s="4" t="inlineStr">
         <is>
-          <t>Pico Truncado</t>
+          <t>Koluel Kayke</t>
         </is>
       </c>
       <c r="D25" s="5" t="n">
-        <v>45771.40826388889</v>
+        <v>45770.76137731481</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>45772.41405092592</v>
+        <v>45770.7769212963</v>
       </c>
       <c r="F25" s="4" t="n">
-        <v>3662</v>
+        <v>224</v>
       </c>
       <c r="G25" s="4" t="inlineStr">
         <is>
-          <t>06:27:50</t>
+          <t>00:22:23</t>
         </is>
       </c>
       <c r="H25" s="4" t="n">
-        <v>11.692</v>
+        <v>1.528</v>
       </c>
       <c r="I25" s="4" t="n">
-        <v>18.11133641241683</v>
+        <v>0.3093282557293622</v>
       </c>
       <c r="J25" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-44900833- -APNSDYME# ENACOM</t>
+          <t>EX-2025-44888593- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K25" s="4" t="inlineStr">
@@ -1438,32 +1438,32 @@
       </c>
       <c r="C26" s="4" t="inlineStr">
         <is>
-          <t>Puerto Deseado</t>
+          <t>Las Heras</t>
         </is>
       </c>
       <c r="D26" s="5" t="n">
-        <v>45775.63364583333</v>
+        <v>45769.6825925926</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>45776.65954861111</v>
+        <v>45770.69950231481</v>
       </c>
       <c r="F26" s="4" t="n">
-        <v>2551</v>
+        <v>3469</v>
       </c>
       <c r="G26" s="4" t="inlineStr">
         <is>
-          <t>05:07:21</t>
+          <t>06:13:06</t>
         </is>
       </c>
       <c r="H26" s="4" t="n">
-        <v>8.297000000000001</v>
+        <v>4.318</v>
       </c>
       <c r="I26" s="4" t="n">
-        <v>9.120424747648924</v>
+        <v>2.470234370621722</v>
       </c>
       <c r="J26" s="4" t="inlineStr">
         <is>
-          <t>EX-2025- 46399962- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-44888902- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K26" s="4" t="inlineStr">
@@ -1485,37 +1485,37 @@
       </c>
       <c r="C27" s="4" t="inlineStr">
         <is>
-          <t>Rio Gallegos</t>
+          <t>Los Antiguos</t>
         </is>
       </c>
       <c r="D27" s="5" t="n">
-        <v>45734.37574074074</v>
+        <v>45769.42946759259</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>45736.7022337963</v>
+        <v>45769.51760416666</v>
       </c>
       <c r="F27" s="4" t="n">
-        <v>10546</v>
+        <v>1085</v>
       </c>
       <c r="G27" s="4" t="inlineStr">
         <is>
-          <t>17:49:33</t>
+          <t>02:02:41</t>
         </is>
       </c>
       <c r="H27" s="4" t="n">
-        <v>12.385</v>
+        <v>2.739</v>
       </c>
       <c r="I27" s="4" t="n">
-        <v>20.32192789083399</v>
+        <v>0.9939326306847305</v>
       </c>
       <c r="J27" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-30586509- -APNSDYME# ENACOM</t>
+          <t>EX-2025-44890916- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K27" s="4" t="inlineStr">
         <is>
-          <t>EF1891</t>
+          <t>EF0391</t>
         </is>
       </c>
     </row>
@@ -1532,32 +1532,32 @@
       </c>
       <c r="C28" s="4" t="inlineStr">
         <is>
-          <t>Río Turbio</t>
+          <t>Perito Moreno</t>
         </is>
       </c>
       <c r="D28" s="5" t="n">
-        <v>45722.77626157407</v>
+        <v>45768.63813657407</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>45723.54744212963</v>
+        <v>45768.7884837963</v>
       </c>
       <c r="F28" s="4" t="n">
-        <v>1596</v>
+        <v>1350</v>
       </c>
       <c r="G28" s="4" t="inlineStr">
         <is>
-          <t>03:40:52</t>
+          <t>02:53:22</t>
         </is>
       </c>
       <c r="H28" s="4" t="n">
-        <v>10.208</v>
+        <v>11.549</v>
       </c>
       <c r="I28" s="4" t="n">
-        <v>13.80556569448233</v>
+        <v>17.67102115722788</v>
       </c>
       <c r="J28" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-26350560- -APNSDYME# ENACOM</t>
+          <t>EX-2025-44890944- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K28" s="4" t="inlineStr">
@@ -1569,42 +1569,42 @@
     <row r="29">
       <c r="A29" s="4" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Comodoro Rivadavia</t>
         </is>
       </c>
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Santa Cruz</t>
         </is>
       </c>
       <c r="C29" s="4" t="inlineStr">
         <is>
-          <t>Colonia Tirolesa</t>
+          <t>Pico Truncado</t>
         </is>
       </c>
       <c r="D29" s="5" t="n">
-        <v>45665.43331018519</v>
+        <v>45771.40826388889</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>45665.51574074074</v>
+        <v>45772.41405092592</v>
       </c>
       <c r="F29" s="4" t="n">
-        <v>1181</v>
+        <v>3662</v>
       </c>
       <c r="G29" s="4" t="inlineStr">
         <is>
-          <t>01:58:42</t>
+          <t>06:27:50</t>
         </is>
       </c>
       <c r="H29" s="4" t="n">
-        <v>3.091</v>
+        <v>11.692</v>
       </c>
       <c r="I29" s="4" t="n">
-        <v>1.265816913461025</v>
+        <v>18.11133641241683</v>
       </c>
       <c r="J29" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-02492718-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-44900833- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K29" s="4" t="inlineStr">
@@ -1616,42 +1616,42 @@
     <row r="30">
       <c r="A30" s="4" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Comodoro Rivadavia</t>
         </is>
       </c>
       <c r="B30" s="4" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Santa Cruz</t>
         </is>
       </c>
       <c r="C30" s="4" t="inlineStr">
         <is>
-          <t>Estación Colonia Tirolesa</t>
+          <t>Puerto Deseado</t>
         </is>
       </c>
       <c r="D30" s="5" t="n">
-        <v>45665.41315972222</v>
+        <v>45775.63364583333</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>45665.42842592593</v>
+        <v>45776.65954861111</v>
       </c>
       <c r="F30" s="4" t="n">
-        <v>224</v>
+        <v>2551</v>
       </c>
       <c r="G30" s="4" t="inlineStr">
         <is>
-          <t>00:21:59</t>
+          <t>05:07:21</t>
         </is>
       </c>
       <c r="H30" s="4" t="n">
-        <v>4.109</v>
+        <v>8.297000000000001</v>
       </c>
       <c r="I30" s="4" t="n">
-        <v>2.23689277452309</v>
+        <v>9.120424747648924</v>
       </c>
       <c r="J30" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-02492607-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025- 46399962- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K30" s="4" t="inlineStr">
@@ -1663,89 +1663,89 @@
     <row r="31">
       <c r="A31" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Comodoro Rivadavia</t>
         </is>
       </c>
       <c r="B31" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Santa Cruz</t>
         </is>
       </c>
       <c r="C31" s="4" t="inlineStr">
         <is>
-          <t>Centenario</t>
+          <t>Rio Gallegos</t>
         </is>
       </c>
       <c r="D31" s="5" t="n">
-        <v>45678.393125</v>
+        <v>45734.37574074074</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>45680.60211805555</v>
+        <v>45736.7022337963</v>
       </c>
       <c r="F31" s="4" t="n">
-        <v>8420</v>
+        <v>10546</v>
       </c>
       <c r="G31" s="4" t="inlineStr">
         <is>
-          <t>12:06:48</t>
+          <t>17:49:33</t>
         </is>
       </c>
       <c r="H31" s="4" t="n">
-        <v>13.145</v>
+        <v>12.385</v>
       </c>
       <c r="I31" s="4" t="n">
-        <v>22.89254439337369</v>
+        <v>20.32192789083399</v>
       </c>
       <c r="J31" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-09027358- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-30586509- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K31" s="4" t="inlineStr">
         <is>
-          <t>EF0391</t>
+          <t>EF1891</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Comodoro Rivadavia</t>
         </is>
       </c>
       <c r="B32" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Santa Cruz</t>
         </is>
       </c>
       <c r="C32" s="4" t="inlineStr">
         <is>
-          <t>Chos Malal</t>
+          <t>Río Turbio</t>
         </is>
       </c>
       <c r="D32" s="5" t="n">
-        <v>45699.39045138889</v>
+        <v>45722.77626157407</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>45699.55277777778</v>
+        <v>45723.54744212963</v>
       </c>
       <c r="F32" s="4" t="n">
-        <v>2767</v>
+        <v>1596</v>
       </c>
       <c r="G32" s="4" t="inlineStr">
         <is>
-          <t>03:53:45</t>
+          <t>03:40:52</t>
         </is>
       </c>
       <c r="H32" s="4" t="n">
-        <v>5.844</v>
+        <v>10.208</v>
       </c>
       <c r="I32" s="4" t="n">
-        <v>4.524736559768742</v>
+        <v>13.80556569448233</v>
       </c>
       <c r="J32" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-20181898- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-26350560- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K32" s="4" t="inlineStr">
@@ -1757,42 +1757,42 @@
     <row r="33">
       <c r="A33" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Córdoba</t>
         </is>
       </c>
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Córdoba</t>
         </is>
       </c>
       <c r="C33" s="4" t="inlineStr">
         <is>
-          <t>Las Lajas</t>
+          <t>Colonia Tirolesa</t>
         </is>
       </c>
       <c r="D33" s="5" t="n">
-        <v>45700.44364583334</v>
+        <v>45665.43331018519</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>45700.53868055555</v>
+        <v>45665.51574074074</v>
       </c>
       <c r="F33" s="4" t="n">
-        <v>2144</v>
+        <v>1181</v>
       </c>
       <c r="G33" s="4" t="inlineStr">
         <is>
-          <t>02:16:51</t>
+          <t>01:58:42</t>
         </is>
       </c>
       <c r="H33" s="4" t="n">
-        <v>3.277</v>
+        <v>3.091</v>
       </c>
       <c r="I33" s="4" t="n">
-        <v>1.422740737610125</v>
+        <v>1.265816913461025</v>
       </c>
       <c r="J33" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-20200350-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-02492718-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K33" s="4" t="inlineStr">
@@ -1804,42 +1804,42 @@
     <row r="34">
       <c r="A34" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Córdoba</t>
         </is>
       </c>
       <c r="B34" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Córdoba</t>
         </is>
       </c>
       <c r="C34" s="4" t="inlineStr">
         <is>
-          <t>Loncopue</t>
+          <t>Estación Colonia Tirolesa</t>
         </is>
       </c>
       <c r="D34" s="5" t="n">
-        <v>45698.57782407408</v>
+        <v>45665.41315972222</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>45698.67151620371</v>
+        <v>45665.42842592593</v>
       </c>
       <c r="F34" s="4" t="n">
-        <v>1400</v>
+        <v>224</v>
       </c>
       <c r="G34" s="4" t="inlineStr">
         <is>
-          <t>02:14:55</t>
+          <t>00:21:59</t>
         </is>
       </c>
       <c r="H34" s="4" t="n">
-        <v>7.203</v>
+        <v>4.109</v>
       </c>
       <c r="I34" s="4" t="n">
-        <v>6.873844664693583</v>
+        <v>2.23689277452309</v>
       </c>
       <c r="J34" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-20278624-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-02492607-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K34" s="4" t="inlineStr">
@@ -1861,32 +1861,32 @@
       </c>
       <c r="C35" s="4" t="inlineStr">
         <is>
-          <t>Plottier</t>
+          <t>Centenario</t>
         </is>
       </c>
       <c r="D35" s="5" t="n">
-        <v>45692.46568287037</v>
+        <v>45678.393125</v>
       </c>
       <c r="E35" s="5" t="n">
-        <v>45695.57134259259</v>
+        <v>45680.60211805555</v>
       </c>
       <c r="F35" s="4" t="n">
-        <v>8602</v>
+        <v>8420</v>
       </c>
       <c r="G35" s="4" t="inlineStr">
         <is>
-          <t>13:05:56</t>
+          <t>12:06:48</t>
         </is>
       </c>
       <c r="H35" s="4" t="n">
-        <v>9.769</v>
+        <v>13.145</v>
       </c>
       <c r="I35" s="4" t="n">
-        <v>12.64366857770164</v>
+        <v>22.89254439337369</v>
       </c>
       <c r="J35" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-20278858-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-09027358- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K35" s="4" t="inlineStr">
@@ -1908,32 +1908,32 @@
       </c>
       <c r="C36" s="4" t="inlineStr">
         <is>
-          <t>San Martín de los Andes</t>
+          <t>Chos Malal</t>
         </is>
       </c>
       <c r="D36" s="5" t="n">
-        <v>45756.63164351852</v>
+        <v>45699.39045138889</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>45757.56960648148</v>
+        <v>45699.55277777778</v>
       </c>
       <c r="F36" s="4" t="n">
-        <v>4021</v>
+        <v>2767</v>
       </c>
       <c r="G36" s="4" t="inlineStr">
         <is>
-          <t>06:04:59</t>
+          <t>03:53:45</t>
         </is>
       </c>
       <c r="H36" s="4" t="n">
-        <v>8.176</v>
+        <v>5.844</v>
       </c>
       <c r="I36" s="4" t="n">
-        <v>8.856347519454705</v>
+        <v>4.524736559768742</v>
       </c>
       <c r="J36" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-39977319- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-20181898- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K36" s="4" t="inlineStr">
@@ -1955,32 +1955,32 @@
       </c>
       <c r="C37" s="4" t="inlineStr">
         <is>
-          <t>Senillosa</t>
+          <t>Las Lajas</t>
         </is>
       </c>
       <c r="D37" s="5" t="n">
-        <v>45741.4528125</v>
+        <v>45700.44364583334</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>45741.58811342593</v>
+        <v>45700.53868055555</v>
       </c>
       <c r="F37" s="4" t="n">
-        <v>2260</v>
+        <v>2144</v>
       </c>
       <c r="G37" s="4" t="inlineStr">
         <is>
-          <t>03:14:50</t>
+          <t>02:16:51</t>
         </is>
       </c>
       <c r="H37" s="4" t="n">
-        <v>6.355</v>
+        <v>3.277</v>
       </c>
       <c r="I37" s="4" t="n">
-        <v>5.350618587883253</v>
+        <v>1.422740737610125</v>
       </c>
       <c r="J37" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-32553095- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-20200350-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K37" s="4" t="inlineStr">
@@ -2002,32 +2002,32 @@
       </c>
       <c r="C38" s="4" t="inlineStr">
         <is>
-          <t>Villa La Angostura</t>
+          <t>Loncopue</t>
         </is>
       </c>
       <c r="D38" s="5" t="n">
-        <v>45758.37885416667</v>
+        <v>45698.57782407408</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>45758.49877314815</v>
+        <v>45698.67151620371</v>
       </c>
       <c r="F38" s="4" t="n">
-        <v>2226</v>
+        <v>1400</v>
       </c>
       <c r="G38" s="4" t="inlineStr">
         <is>
-          <t>02:52:41</t>
+          <t>02:14:55</t>
         </is>
       </c>
       <c r="H38" s="4" t="n">
-        <v>6.26</v>
+        <v>7.203</v>
       </c>
       <c r="I38" s="4" t="n">
-        <v>5.19184299456393</v>
+        <v>6.873844664693583</v>
       </c>
       <c r="J38" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-39977661- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-20278624-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K38" s="4" t="inlineStr">
@@ -2049,32 +2049,32 @@
       </c>
       <c r="C39" s="4" t="inlineStr">
         <is>
-          <t>Zapala</t>
+          <t>Plottier</t>
         </is>
       </c>
       <c r="D39" s="5" t="n">
-        <v>45700.61767361111</v>
+        <v>45692.46568287037</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>45701.60255787037</v>
+        <v>45695.57134259259</v>
       </c>
       <c r="F39" s="4" t="n">
-        <v>5900</v>
+        <v>8602</v>
       </c>
       <c r="G39" s="4" t="inlineStr">
         <is>
-          <t>06:48:10</t>
+          <t>13:05:56</t>
         </is>
       </c>
       <c r="H39" s="4" t="n">
-        <v>7.476</v>
+        <v>9.769</v>
       </c>
       <c r="I39" s="4" t="n">
-        <v>7.404768229433365</v>
+        <v>12.64366857770164</v>
       </c>
       <c r="J39" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-20279172-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-20278858-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K39" s="4" t="inlineStr">
@@ -2091,33 +2091,37 @@
       </c>
       <c r="B40" s="4" t="inlineStr">
         <is>
-          <t>Río Negro</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="C40" s="4" t="inlineStr">
         <is>
-          <t>Allen</t>
-        </is>
-      </c>
-      <c r="D40" s="4" t="inlineStr"/>
-      <c r="E40" s="4" t="inlineStr"/>
+          <t>San Martín de los Andes</t>
+        </is>
+      </c>
+      <c r="D40" s="5" t="n">
+        <v>45756.63164351852</v>
+      </c>
+      <c r="E40" s="5" t="n">
+        <v>45757.56960648148</v>
+      </c>
       <c r="F40" s="4" t="n">
-        <v>5422</v>
+        <v>4021</v>
       </c>
       <c r="G40" s="4" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>06:04:59</t>
         </is>
       </c>
       <c r="H40" s="4" t="n">
-        <v>10.342</v>
+        <v>8.176</v>
       </c>
       <c r="I40" s="4" t="n">
-        <v>14.17039482548629</v>
+        <v>8.856347519454705</v>
       </c>
       <c r="J40" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-62134249- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-39977319- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K40" s="4" t="inlineStr">
@@ -2129,42 +2133,42 @@
     <row r="41">
       <c r="A41" s="4" t="inlineStr">
         <is>
-          <t>Posadas</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="B41" s="4" t="inlineStr">
         <is>
-          <t>Chaco</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="C41" s="4" t="inlineStr">
         <is>
-          <t>Barranqueras</t>
+          <t>Senillosa</t>
         </is>
       </c>
       <c r="D41" s="5" t="n">
-        <v>45812.55844907407</v>
+        <v>45741.4528125</v>
       </c>
       <c r="E41" s="5" t="n">
-        <v>45813.55945601852</v>
+        <v>45741.58811342593</v>
       </c>
       <c r="F41" s="4" t="n">
-        <v>1542</v>
+        <v>2260</v>
       </c>
       <c r="G41" s="4" t="inlineStr">
         <is>
-          <t>03:51:20</t>
+          <t>03:14:50</t>
         </is>
       </c>
       <c r="H41" s="4" t="n">
-        <v>11.927</v>
+        <v>6.355</v>
       </c>
       <c r="I41" s="4" t="n">
-        <v>18.84670022206126</v>
+        <v>5.350618587883253</v>
       </c>
       <c r="J41" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-97804852-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-32553095- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K41" s="4" t="inlineStr">
@@ -2176,42 +2180,42 @@
     <row r="42">
       <c r="A42" s="4" t="inlineStr">
         <is>
-          <t>Posadas</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="B42" s="4" t="inlineStr">
         <is>
-          <t>Chaco</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="C42" s="4" t="inlineStr">
         <is>
-          <t>Basail</t>
+          <t>Villa La Angostura</t>
         </is>
       </c>
       <c r="D42" s="5" t="n">
-        <v>45916.46837962963</v>
+        <v>45758.37885416667</v>
       </c>
       <c r="E42" s="5" t="n">
-        <v>45916.5103125</v>
+        <v>45758.49877314815</v>
       </c>
       <c r="F42" s="4" t="n">
-        <v>811</v>
+        <v>2226</v>
       </c>
       <c r="G42" s="4" t="inlineStr">
         <is>
-          <t>01:00:23</t>
+          <t>02:52:41</t>
         </is>
       </c>
       <c r="H42" s="4" t="n">
-        <v>8.038</v>
+        <v>6.26</v>
       </c>
       <c r="I42" s="4" t="n">
-        <v>8.559903878116309</v>
+        <v>5.19184299456393</v>
       </c>
       <c r="J42" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-105147378-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-39977661- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K42" s="4" t="inlineStr">
@@ -2223,42 +2227,42 @@
     <row r="43">
       <c r="A43" s="4" t="inlineStr">
         <is>
-          <t>Posadas</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="B43" s="4" t="inlineStr">
         <is>
-          <t>Chaco</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="C43" s="4" t="inlineStr">
         <is>
-          <t>Corzuela</t>
+          <t>Zapala</t>
         </is>
       </c>
       <c r="D43" s="5" t="n">
-        <v>45820.53369212963</v>
+        <v>45700.61767361111</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>45820.58216435185</v>
+        <v>45701.60255787037</v>
       </c>
       <c r="F43" s="4" t="n">
-        <v>799</v>
+        <v>5900</v>
       </c>
       <c r="G43" s="4" t="inlineStr">
         <is>
-          <t>01:09:48</t>
+          <t>06:48:10</t>
         </is>
       </c>
       <c r="H43" s="4" t="n">
-        <v>2.94</v>
+        <v>7.476</v>
       </c>
       <c r="I43" s="4" t="n">
-        <v>1.145163625938123</v>
+        <v>7.404768229433365</v>
       </c>
       <c r="J43" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73262047-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-20279172-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K43" s="4" t="inlineStr">
@@ -2270,42 +2274,42 @@
     <row r="44">
       <c r="A44" s="4" t="inlineStr">
         <is>
-          <t>Posadas</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="B44" s="4" t="inlineStr">
         <is>
-          <t>Chaco</t>
+          <t>Río Negro</t>
         </is>
       </c>
       <c r="C44" s="4" t="inlineStr">
         <is>
-          <t>Fontana</t>
+          <t>Allen</t>
         </is>
       </c>
       <c r="D44" s="5" t="n">
-        <v>45918.52649305556</v>
+        <v>45742.42247685185</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>45918.56483796296</v>
+        <v>45813.52212962963</v>
       </c>
       <c r="F44" s="4" t="n">
-        <v>687</v>
+        <v>5422</v>
       </c>
       <c r="G44" s="4" t="inlineStr">
         <is>
-          <t>00:55:13</t>
+          <t>07:23:01</t>
         </is>
       </c>
       <c r="H44" s="4" t="n">
-        <v>6.305</v>
+        <v>10.342</v>
       </c>
       <c r="I44" s="4" t="n">
-        <v>5.26675439064844</v>
+        <v>14.17039482548629</v>
       </c>
       <c r="J44" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-105147260-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-62134249- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K44" s="4" t="inlineStr">
@@ -2327,32 +2331,32 @@
       </c>
       <c r="C45" s="4" t="inlineStr">
         <is>
-          <t>General Pinedo</t>
+          <t>Barranqueras</t>
         </is>
       </c>
       <c r="D45" s="5" t="n">
-        <v>45820.41590277778</v>
+        <v>45812.55844907407</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>45820.45375</v>
+        <v>45813.55945601852</v>
       </c>
       <c r="F45" s="4" t="n">
-        <v>586</v>
+        <v>1542</v>
       </c>
       <c r="G45" s="4" t="inlineStr">
         <is>
-          <t>00:54:30</t>
+          <t>03:51:20</t>
         </is>
       </c>
       <c r="H45" s="4" t="n">
-        <v>5.347</v>
+        <v>11.927</v>
       </c>
       <c r="I45" s="4" t="n">
-        <v>3.787854185466004</v>
+        <v>18.84670022206126</v>
       </c>
       <c r="J45" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73254360-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-97804852-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K45" s="4" t="inlineStr">
@@ -2374,32 +2378,32 @@
       </c>
       <c r="C46" s="4" t="inlineStr">
         <is>
-          <t>General San Martín</t>
+          <t>Basail</t>
         </is>
       </c>
       <c r="D46" s="5" t="n">
-        <v>45818.56168981481</v>
+        <v>45916.46837962963</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>45818.70513888889</v>
+        <v>45916.5103125</v>
       </c>
       <c r="F46" s="4" t="n">
-        <v>914</v>
+        <v>811</v>
       </c>
       <c r="G46" s="4" t="inlineStr">
         <is>
-          <t>01:35:41</t>
+          <t>01:00:23</t>
         </is>
       </c>
       <c r="H46" s="4" t="n">
-        <v>5.561</v>
+        <v>8.038</v>
       </c>
       <c r="I46" s="4" t="n">
-        <v>4.097119907386369</v>
+        <v>8.559903878116309</v>
       </c>
       <c r="J46" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73254137-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-105147378-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K46" s="4" t="inlineStr">
@@ -2421,32 +2425,32 @@
       </c>
       <c r="C47" s="4" t="inlineStr">
         <is>
-          <t>Ituzaingo</t>
+          <t>Corzuela</t>
         </is>
       </c>
       <c r="D47" s="5" t="n">
-        <v>45831.48724537037</v>
+        <v>45820.53369212963</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>45831.56583333333</v>
+        <v>45820.58216435185</v>
       </c>
       <c r="F47" s="4" t="n">
-        <v>1182</v>
+        <v>799</v>
       </c>
       <c r="G47" s="4" t="inlineStr">
         <is>
-          <t>01:53:10</t>
+          <t>01:09:48</t>
         </is>
       </c>
       <c r="H47" s="4" t="n">
-        <v>9.388999999999999</v>
+        <v>2.94</v>
       </c>
       <c r="I47" s="4" t="n">
-        <v>11.67915876658421</v>
+        <v>1.145163625938123</v>
       </c>
       <c r="J47" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73252694-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-73262047-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K47" s="4" t="inlineStr">
@@ -2468,32 +2472,32 @@
       </c>
       <c r="C48" s="4" t="inlineStr">
         <is>
-          <t>Las Breñas</t>
+          <t>Fontana</t>
         </is>
       </c>
       <c r="D48" s="5" t="n">
-        <v>45819.71625</v>
+        <v>45918.52649305556</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>45819.76673611111</v>
+        <v>45918.56483796296</v>
       </c>
       <c r="F48" s="4" t="n">
-        <v>954</v>
+        <v>687</v>
       </c>
       <c r="G48" s="4" t="inlineStr">
         <is>
-          <t>01:12:42</t>
+          <t>00:55:13</t>
         </is>
       </c>
       <c r="H48" s="4" t="n">
-        <v>3.477</v>
+        <v>6.305</v>
       </c>
       <c r="I48" s="4" t="n">
-        <v>1.60170401979778</v>
+        <v>5.26675439064844</v>
       </c>
       <c r="J48" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73253915-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-105147260-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K48" s="4" t="inlineStr">
@@ -2515,32 +2519,32 @@
       </c>
       <c r="C49" s="4" t="inlineStr">
         <is>
-          <t>Machagai</t>
+          <t>General Pinedo</t>
         </is>
       </c>
       <c r="D49" s="5" t="n">
-        <v>45819.50070601852</v>
+        <v>45820.41590277778</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>45819.56872685185</v>
+        <v>45820.45375</v>
       </c>
       <c r="F49" s="4" t="n">
-        <v>794</v>
+        <v>586</v>
       </c>
       <c r="G49" s="4" t="inlineStr">
         <is>
-          <t>01:37:57</t>
+          <t>00:54:30</t>
         </is>
       </c>
       <c r="H49" s="4" t="n">
-        <v>3.329</v>
+        <v>5.347</v>
       </c>
       <c r="I49" s="4" t="n">
-        <v>1.468251571923751</v>
+        <v>3.787854185466004</v>
       </c>
       <c r="J49" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73253720-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-73254360-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K49" s="4" t="inlineStr">
@@ -2562,32 +2566,32 @@
       </c>
       <c r="C50" s="4" t="inlineStr">
         <is>
-          <t>Presidencia de la Plaza</t>
+          <t>General San Martín</t>
         </is>
       </c>
       <c r="D50" s="5" t="n">
-        <v>45896.461875</v>
+        <v>45818.56168981481</v>
       </c>
       <c r="E50" s="5" t="n">
-        <v>45896.52564814815</v>
+        <v>45818.70513888889</v>
       </c>
       <c r="F50" s="4" t="n">
-        <v>865</v>
+        <v>914</v>
       </c>
       <c r="G50" s="4" t="inlineStr">
         <is>
-          <t>01:31:50</t>
+          <t>01:35:41</t>
         </is>
       </c>
       <c r="H50" s="4" t="n">
-        <v>3.203</v>
+        <v>5.561</v>
       </c>
       <c r="I50" s="4" t="n">
-        <v>1.359210627249875</v>
+        <v>4.097119907386369</v>
       </c>
       <c r="J50" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-97797640-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-73254137-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K50" s="4" t="inlineStr">
@@ -2609,32 +2613,32 @@
       </c>
       <c r="C51" s="4" t="inlineStr">
         <is>
-          <t>Puerto Vilelas</t>
+          <t>Ituzaingo</t>
         </is>
       </c>
       <c r="D51" s="5" t="n">
-        <v>45812.42873842592</v>
+        <v>45831.48724537037</v>
       </c>
       <c r="E51" s="5" t="n">
-        <v>45812.53604166667</v>
+        <v>45831.56583333333</v>
       </c>
       <c r="F51" s="4" t="n">
-        <v>975</v>
+        <v>1182</v>
       </c>
       <c r="G51" s="4" t="inlineStr">
         <is>
-          <t>02:16:46</t>
+          <t>01:53:10</t>
         </is>
       </c>
       <c r="H51" s="4" t="n">
-        <v>13.864</v>
+        <v>9.388999999999999</v>
       </c>
       <c r="I51" s="4" t="n">
-        <v>25.46536958474769</v>
+        <v>11.67915876658421</v>
       </c>
       <c r="J51" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73253473-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-73252694-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K51" s="4" t="inlineStr">
@@ -2656,32 +2660,32 @@
       </c>
       <c r="C52" s="4" t="inlineStr">
         <is>
-          <t>Quitipili</t>
+          <t>Las Breñas</t>
         </is>
       </c>
       <c r="D52" s="5" t="n">
-        <v>45896.55892361111</v>
+        <v>45819.71625</v>
       </c>
       <c r="E52" s="5" t="n">
-        <v>45896.65435185185</v>
+        <v>45819.76673611111</v>
       </c>
       <c r="F52" s="4" t="n">
-        <v>1404</v>
+        <v>954</v>
       </c>
       <c r="G52" s="4" t="inlineStr">
         <is>
-          <t>02:17:25</t>
+          <t>01:12:42</t>
         </is>
       </c>
       <c r="H52" s="4" t="n">
-        <v>3.1</v>
+        <v>3.477</v>
       </c>
       <c r="I52" s="4" t="n">
-        <v>1.273198950120941</v>
+        <v>1.60170401979778</v>
       </c>
       <c r="J52" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-97797814-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-73253915-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K52" s="4" t="inlineStr">
@@ -2703,32 +2707,32 @@
       </c>
       <c r="C53" s="4" t="inlineStr">
         <is>
-          <t>Resistencia</t>
+          <t>Machagai</t>
         </is>
       </c>
       <c r="D53" s="5" t="n">
-        <v>45917.46174768519</v>
+        <v>45819.50070601852</v>
       </c>
       <c r="E53" s="5" t="n">
-        <v>45918.5246875</v>
+        <v>45819.56872685185</v>
       </c>
       <c r="F53" s="4" t="n">
-        <v>4525</v>
+        <v>794</v>
       </c>
       <c r="G53" s="4" t="inlineStr">
         <is>
-          <t>07:29:04</t>
+          <t>01:37:57</t>
         </is>
       </c>
       <c r="H53" s="4" t="n">
-        <v>9.226000000000001</v>
+        <v>3.329</v>
       </c>
       <c r="I53" s="4" t="n">
-        <v>11.27716110285792</v>
+        <v>1.468251571923751</v>
       </c>
       <c r="J53" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-105147001-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-73253720-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K53" s="4" t="inlineStr">
@@ -2750,32 +2754,32 @@
       </c>
       <c r="C54" s="4" t="inlineStr">
         <is>
-          <t>Roque Saenz Peña</t>
+          <t>Presidencia de la Plaza</t>
         </is>
       </c>
       <c r="D54" s="5" t="n">
-        <v>45820.65457175926</v>
+        <v>45896.461875</v>
       </c>
       <c r="E54" s="5" t="n">
-        <v>45820.71850694445</v>
+        <v>45896.52564814815</v>
       </c>
       <c r="F54" s="4" t="n">
-        <v>1139</v>
+        <v>865</v>
       </c>
       <c r="G54" s="4" t="inlineStr">
         <is>
-          <t>01:32:04</t>
+          <t>01:31:50</t>
         </is>
       </c>
       <c r="H54" s="4" t="n">
-        <v>4.777</v>
+        <v>3.203</v>
       </c>
       <c r="I54" s="4" t="n">
-        <v>3.023314776778812</v>
+        <v>1.359210627249875</v>
       </c>
       <c r="J54" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73253145-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-97797640-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K54" s="4" t="inlineStr">
@@ -2797,32 +2801,32 @@
       </c>
       <c r="C55" s="4" t="inlineStr">
         <is>
-          <t>Villa Ángela</t>
+          <t>Puerto Vilelas</t>
         </is>
       </c>
       <c r="D55" s="5" t="n">
-        <v>45897.51820601852</v>
+        <v>45812.42873842592</v>
       </c>
       <c r="E55" s="5" t="n">
-        <v>45897.66859953704</v>
+        <v>45812.53604166667</v>
       </c>
       <c r="F55" s="4" t="n">
-        <v>2380</v>
+        <v>975</v>
       </c>
       <c r="G55" s="4" t="inlineStr">
         <is>
-          <t>03:36:34</t>
+          <t>02:16:46</t>
         </is>
       </c>
       <c r="H55" s="4" t="n">
-        <v>7.56</v>
+        <v>13.864</v>
       </c>
       <c r="I55" s="4" t="n">
-        <v>7.572102342937794</v>
+        <v>25.46536958474769</v>
       </c>
       <c r="J55" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-97798907-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-73253473-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K55" s="4" t="inlineStr">
@@ -2839,37 +2843,37 @@
       </c>
       <c r="B56" s="4" t="inlineStr">
         <is>
-          <t>Corrientes</t>
+          <t>Chaco</t>
         </is>
       </c>
       <c r="C56" s="4" t="inlineStr">
         <is>
-          <t>Corrientes</t>
+          <t>Quitipili</t>
         </is>
       </c>
       <c r="D56" s="5" t="n">
-        <v>45832.40711805555</v>
+        <v>45896.55892361111</v>
       </c>
       <c r="E56" s="5" t="n">
-        <v>45833.658125</v>
+        <v>45896.65435185185</v>
       </c>
       <c r="F56" s="4" t="n">
-        <v>7411</v>
+        <v>1404</v>
       </c>
       <c r="G56" s="4" t="inlineStr">
         <is>
-          <t>12:49:16</t>
+          <t>02:17:25</t>
         </is>
       </c>
       <c r="H56" s="4" t="n">
-        <v>12.527</v>
+        <v>3.1</v>
       </c>
       <c r="I56" s="4" t="n">
-        <v>20.79060077104716</v>
+        <v>1.273198950120941</v>
       </c>
       <c r="J56" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73252918-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-97797814-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K56" s="4" t="inlineStr">
@@ -2886,37 +2890,37 @@
       </c>
       <c r="B57" s="4" t="inlineStr">
         <is>
-          <t>Corrientes</t>
+          <t>Chaco</t>
         </is>
       </c>
       <c r="C57" s="4" t="inlineStr">
         <is>
-          <t>Ituzaingo</t>
+          <t>Resistencia</t>
         </is>
       </c>
       <c r="D57" s="5" t="n">
-        <v>45831.48724537037</v>
+        <v>45917.46174768519</v>
       </c>
       <c r="E57" s="5" t="n">
-        <v>45831.56583333333</v>
+        <v>45918.5246875</v>
       </c>
       <c r="F57" s="4" t="n">
-        <v>1182</v>
+        <v>4525</v>
       </c>
       <c r="G57" s="4" t="inlineStr">
         <is>
-          <t>01:53:10</t>
+          <t>07:29:04</t>
         </is>
       </c>
       <c r="H57" s="4" t="n">
-        <v>9.388999999999999</v>
+        <v>9.226000000000001</v>
       </c>
       <c r="I57" s="4" t="n">
-        <v>11.67915876658421</v>
+        <v>11.27716110285792</v>
       </c>
       <c r="J57" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73252694-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-105147001-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K57" s="4" t="inlineStr">
@@ -2933,37 +2937,37 @@
       </c>
       <c r="B58" s="4" t="inlineStr">
         <is>
-          <t>Corrientes</t>
+          <t>Chaco</t>
         </is>
       </c>
       <c r="C58" s="4" t="inlineStr">
         <is>
-          <t>Paso de la Patria</t>
+          <t>Roque Saenz Peña</t>
         </is>
       </c>
       <c r="D58" s="5" t="n">
-        <v>45831.68550925926</v>
+        <v>45820.65457175926</v>
       </c>
       <c r="E58" s="5" t="n">
-        <v>45831.73684027778</v>
+        <v>45820.71850694445</v>
       </c>
       <c r="F58" s="4" t="n">
-        <v>828</v>
+        <v>1139</v>
       </c>
       <c r="G58" s="4" t="inlineStr">
         <is>
-          <t>01:13:55</t>
+          <t>01:32:04</t>
         </is>
       </c>
       <c r="H58" s="4" t="n">
-        <v>3.111</v>
+        <v>4.777</v>
       </c>
       <c r="I58" s="4" t="n">
-        <v>1.282250586486312</v>
+        <v>3.023314776778812</v>
       </c>
       <c r="J58" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73252434-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-73253145-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K58" s="4" t="inlineStr">
@@ -2980,37 +2984,37 @@
       </c>
       <c r="B59" s="4" t="inlineStr">
         <is>
-          <t>Formosa</t>
+          <t>Chaco</t>
         </is>
       </c>
       <c r="C59" s="4" t="inlineStr">
         <is>
-          <t>Formosa</t>
+          <t>Villa Ángela</t>
         </is>
       </c>
       <c r="D59" s="5" t="n">
-        <v>45847.47630787037</v>
+        <v>45897.51820601852</v>
       </c>
       <c r="E59" s="5" t="n">
-        <v>45848.71959490741</v>
+        <v>45897.66859953704</v>
       </c>
       <c r="F59" s="4" t="n">
-        <v>5553</v>
+        <v>2380</v>
       </c>
       <c r="G59" s="4" t="inlineStr">
         <is>
-          <t>10:32:42</t>
+          <t>03:36:34</t>
         </is>
       </c>
       <c r="H59" s="4" t="n">
-        <v>8.835000000000001</v>
+        <v>7.56</v>
       </c>
       <c r="I59" s="4" t="n">
-        <v>10.34155847235734</v>
+        <v>7.572102342937794</v>
       </c>
       <c r="J59" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-77142320-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-97798907-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K59" s="4" t="inlineStr">
@@ -3027,37 +3031,37 @@
       </c>
       <c r="B60" s="4" t="inlineStr">
         <is>
-          <t>Formosa</t>
+          <t>Corrientes</t>
         </is>
       </c>
       <c r="C60" s="4" t="inlineStr">
         <is>
-          <t>Laguna Blanca</t>
+          <t>Corrientes</t>
         </is>
       </c>
       <c r="D60" s="5" t="n">
-        <v>45846.4572337963</v>
+        <v>45832.40711805555</v>
       </c>
       <c r="E60" s="5" t="n">
-        <v>45846.50842592592</v>
+        <v>45833.658125</v>
       </c>
       <c r="F60" s="4" t="n">
-        <v>610</v>
+        <v>7411</v>
       </c>
       <c r="G60" s="4" t="inlineStr">
         <is>
-          <t>01:13:43</t>
+          <t>12:49:16</t>
         </is>
       </c>
       <c r="H60" s="4" t="n">
-        <v>2.874</v>
+        <v>12.527</v>
       </c>
       <c r="I60" s="4" t="n">
-        <v>1.094325229066509</v>
+        <v>20.79060077104716</v>
       </c>
       <c r="J60" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-77142546-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-73252918-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K60" s="4" t="inlineStr">
@@ -3069,139 +3073,327 @@
     <row r="61">
       <c r="A61" s="4" t="inlineStr">
         <is>
-          <t>Salta</t>
+          <t>Posadas</t>
         </is>
       </c>
       <c r="B61" s="4" t="inlineStr">
         <is>
-          <t>Jujuy</t>
+          <t>Corrientes</t>
         </is>
       </c>
       <c r="C61" s="4" t="inlineStr">
         <is>
-          <t>San Pablo de Reyes</t>
+          <t>Ituzaingo</t>
         </is>
       </c>
       <c r="D61" s="5" t="n">
-        <v>45734.39631944444</v>
+        <v>45831.48724537037</v>
       </c>
       <c r="E61" s="5" t="n">
-        <v>45734.41811342593</v>
+        <v>45831.56583333333</v>
       </c>
       <c r="F61" s="4" t="n">
-        <v>260</v>
+        <v>1182</v>
       </c>
       <c r="G61" s="4" t="inlineStr">
         <is>
-          <t>00:25:35</t>
+          <t>01:53:10</t>
         </is>
       </c>
       <c r="H61" s="4" t="n">
-        <v>4.246</v>
+        <v>9.388999999999999</v>
       </c>
       <c r="I61" s="4" t="n">
-        <v>2.388541898380706</v>
+        <v>11.67915876658421</v>
       </c>
       <c r="J61" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-33150525-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-73252694-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K61" s="4" t="inlineStr">
         <is>
-          <t>EF1891</t>
+          <t>EF0391</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="4" t="inlineStr">
         <is>
-          <t>Salta</t>
+          <t>Posadas</t>
         </is>
       </c>
       <c r="B62" s="4" t="inlineStr">
         <is>
-          <t>Jujuy</t>
+          <t>Corrientes</t>
         </is>
       </c>
       <c r="C62" s="4" t="inlineStr">
         <is>
-          <t>San Salvador de Jujuy</t>
+          <t>Paso de la Patria</t>
         </is>
       </c>
       <c r="D62" s="5" t="n">
-        <v>45734.45050925926</v>
+        <v>45831.68550925926</v>
       </c>
       <c r="E62" s="5" t="n">
-        <v>45736.80579861111</v>
+        <v>45831.73684027778</v>
       </c>
       <c r="F62" s="4" t="n">
-        <v>7808</v>
+        <v>828</v>
       </c>
       <c r="G62" s="4" t="inlineStr">
         <is>
-          <t>17:51:37</t>
+          <t>01:13:55</t>
         </is>
       </c>
       <c r="H62" s="4" t="n">
-        <v>16.837</v>
+        <v>3.111</v>
       </c>
       <c r="I62" s="4" t="n">
-        <v>37.55798705788629</v>
+        <v>1.282250586486312</v>
       </c>
       <c r="J62" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-101525989- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-73252434-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K62" s="4" t="inlineStr">
         <is>
-          <t>EF0391, EF1891</t>
+          <t>EF0391</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="4" t="inlineStr">
         <is>
+          <t>Posadas</t>
+        </is>
+      </c>
+      <c r="B63" s="4" t="inlineStr">
+        <is>
+          <t>Formosa</t>
+        </is>
+      </c>
+      <c r="C63" s="4" t="inlineStr">
+        <is>
+          <t>Formosa</t>
+        </is>
+      </c>
+      <c r="D63" s="5" t="n">
+        <v>45847.47630787037</v>
+      </c>
+      <c r="E63" s="5" t="n">
+        <v>45848.71959490741</v>
+      </c>
+      <c r="F63" s="4" t="n">
+        <v>5553</v>
+      </c>
+      <c r="G63" s="4" t="inlineStr">
+        <is>
+          <t>10:32:42</t>
+        </is>
+      </c>
+      <c r="H63" s="4" t="n">
+        <v>8.835000000000001</v>
+      </c>
+      <c r="I63" s="4" t="n">
+        <v>10.34155847235734</v>
+      </c>
+      <c r="J63" s="4" t="inlineStr">
+        <is>
+          <t>EX-2025-77142320-   -APN-SDYME#ENACOM</t>
+        </is>
+      </c>
+      <c r="K63" s="4" t="inlineStr">
+        <is>
+          <t>EF0391</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="4" t="inlineStr">
+        <is>
+          <t>Posadas</t>
+        </is>
+      </c>
+      <c r="B64" s="4" t="inlineStr">
+        <is>
+          <t>Formosa</t>
+        </is>
+      </c>
+      <c r="C64" s="4" t="inlineStr">
+        <is>
+          <t>Laguna Blanca</t>
+        </is>
+      </c>
+      <c r="D64" s="5" t="n">
+        <v>45846.4572337963</v>
+      </c>
+      <c r="E64" s="5" t="n">
+        <v>45846.50842592592</v>
+      </c>
+      <c r="F64" s="4" t="n">
+        <v>610</v>
+      </c>
+      <c r="G64" s="4" t="inlineStr">
+        <is>
+          <t>01:13:43</t>
+        </is>
+      </c>
+      <c r="H64" s="4" t="n">
+        <v>2.874</v>
+      </c>
+      <c r="I64" s="4" t="n">
+        <v>1.094325229066509</v>
+      </c>
+      <c r="J64" s="4" t="inlineStr">
+        <is>
+          <t>EX-2025-77142546-   -APN-SDYME#ENACOM</t>
+        </is>
+      </c>
+      <c r="K64" s="4" t="inlineStr">
+        <is>
+          <t>EF0391</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="4" t="inlineStr">
+        <is>
           <t>Salta</t>
         </is>
       </c>
-      <c r="B63" s="4" t="inlineStr">
+      <c r="B65" s="4" t="inlineStr">
         <is>
           <t>Jujuy</t>
         </is>
       </c>
-      <c r="C63" s="4" t="inlineStr">
+      <c r="C65" s="4" t="inlineStr">
+        <is>
+          <t>San Pablo de Reyes</t>
+        </is>
+      </c>
+      <c r="D65" s="5" t="n">
+        <v>45734.39631944444</v>
+      </c>
+      <c r="E65" s="5" t="n">
+        <v>45734.41811342593</v>
+      </c>
+      <c r="F65" s="4" t="n">
+        <v>260</v>
+      </c>
+      <c r="G65" s="4" t="inlineStr">
+        <is>
+          <t>00:25:35</t>
+        </is>
+      </c>
+      <c r="H65" s="4" t="n">
+        <v>4.246</v>
+      </c>
+      <c r="I65" s="4" t="n">
+        <v>2.388541898380706</v>
+      </c>
+      <c r="J65" s="4" t="inlineStr">
+        <is>
+          <t>EX-2025-33150525-   -APN-SDYME#ENACOM</t>
+        </is>
+      </c>
+      <c r="K65" s="4" t="inlineStr">
+        <is>
+          <t>EF1891</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="4" t="inlineStr">
+        <is>
+          <t>Salta</t>
+        </is>
+      </c>
+      <c r="B66" s="4" t="inlineStr">
+        <is>
+          <t>Jujuy</t>
+        </is>
+      </c>
+      <c r="C66" s="4" t="inlineStr">
+        <is>
+          <t>San Salvador de Jujuy</t>
+        </is>
+      </c>
+      <c r="D66" s="5" t="n">
+        <v>45734.45050925926</v>
+      </c>
+      <c r="E66" s="5" t="n">
+        <v>45736.80579861111</v>
+      </c>
+      <c r="F66" s="4" t="n">
+        <v>7808</v>
+      </c>
+      <c r="G66" s="4" t="inlineStr">
+        <is>
+          <t>17:51:37</t>
+        </is>
+      </c>
+      <c r="H66" s="4" t="n">
+        <v>16.837</v>
+      </c>
+      <c r="I66" s="4" t="n">
+        <v>37.55798705788629</v>
+      </c>
+      <c r="J66" s="4" t="inlineStr">
+        <is>
+          <t>EX-2025-101525989- -APN-SDYME#ENACOM</t>
+        </is>
+      </c>
+      <c r="K66" s="4" t="inlineStr">
+        <is>
+          <t>EF0391, EF1891</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="4" t="inlineStr">
+        <is>
+          <t>Salta</t>
+        </is>
+      </c>
+      <c r="B67" s="4" t="inlineStr">
+        <is>
+          <t>Jujuy</t>
+        </is>
+      </c>
+      <c r="C67" s="4" t="inlineStr">
         <is>
           <t>Villa Jardín de Reyes</t>
         </is>
       </c>
-      <c r="D63" s="5" t="n">
+      <c r="D67" s="5" t="n">
         <v>45733.61721064815</v>
       </c>
-      <c r="E63" s="5" t="n">
+      <c r="E67" s="5" t="n">
         <v>45733.67739583334</v>
       </c>
-      <c r="F63" s="4" t="n">
+      <c r="F67" s="4" t="n">
         <v>545</v>
       </c>
-      <c r="G63" s="4" t="inlineStr">
+      <c r="G67" s="4" t="inlineStr">
         <is>
           <t>01:26:40</t>
         </is>
       </c>
-      <c r="H63" s="4" t="n">
+      <c r="H67" s="4" t="n">
         <v>2.843</v>
       </c>
-      <c r="I63" s="4" t="n">
+      <c r="I67" s="4" t="n">
         <v>1.070844976170247</v>
       </c>
-      <c r="J63" s="4" t="inlineStr">
+      <c r="J67" s="4" t="inlineStr">
         <is>
           <t>EX-2025-33162392-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
-      <c r="K63" s="4" t="inlineStr">
+      <c r="K67" s="4" t="inlineStr">
         <is>
           <t>EF1891</t>
         </is>

</xml_diff>

<commit_message>
Estilo visual al hightop
</commit_message>
<xml_diff>
--- a/resumen_localidades.xlsx
+++ b/resumen_localidades.xlsx
@@ -467,7 +467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A6:K67"/>
+  <dimension ref="A6:K80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,32 +545,32 @@
       </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
-          <t>Cholila</t>
+          <t>28 de Julio</t>
         </is>
       </c>
       <c r="D7" s="5" t="n">
-        <v>45923.45476851852</v>
+        <v>45875.45162037037</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>45923.4960300926</v>
+        <v>45875.46636574074</v>
       </c>
       <c r="F7" s="4" t="n">
-        <v>710</v>
+        <v>231</v>
       </c>
       <c r="G7" s="4" t="inlineStr">
         <is>
-          <t>00:59:25</t>
+          <t>00:21:14</t>
         </is>
       </c>
       <c r="H7" s="4" t="n">
-        <v>1.46</v>
+        <v>1.462</v>
       </c>
       <c r="I7" s="4" t="n">
-        <v>0.2824090407989382</v>
+        <v>0.2831832941459213</v>
       </c>
       <c r="J7" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-107254049- -APNSDYME# ENACOM</t>
+          <t>EX- 2025-86907545- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K7" s="4" t="inlineStr">
@@ -592,32 +592,32 @@
       </c>
       <c r="C8" s="4" t="inlineStr">
         <is>
-          <t>El Hoyo</t>
+          <t>Camarones</t>
         </is>
       </c>
       <c r="D8" s="5" t="n">
-        <v>45923.65008101852</v>
+        <v>45873.5115625</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>45923.71108796296</v>
+        <v>45873.55052083333</v>
       </c>
       <c r="F8" s="4" t="n">
-        <v>917</v>
+        <v>530</v>
       </c>
       <c r="G8" s="4" t="inlineStr">
         <is>
-          <t>01:27:51</t>
+          <t>00:56:06</t>
         </is>
       </c>
       <c r="H8" s="4" t="n">
-        <v>5.38</v>
+        <v>2.137</v>
       </c>
       <c r="I8" s="4" t="n">
-        <v>3.834753349831483</v>
+        <v>0.6050369923251673</v>
       </c>
       <c r="J8" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-107270163- -APNSDYME# ENACOM</t>
+          <t>EX-2025-86908010- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K8" s="4" t="inlineStr">
@@ -639,32 +639,32 @@
       </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
-          <t>El Maiten</t>
+          <t>Cholila</t>
         </is>
       </c>
       <c r="D9" s="5" t="n">
-        <v>45924.47306712963</v>
+        <v>45923.45476851852</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>45924.54931712963</v>
+        <v>45923.4960300926</v>
       </c>
       <c r="F9" s="4" t="n">
-        <v>1042</v>
+        <v>710</v>
       </c>
       <c r="G9" s="4" t="inlineStr">
         <is>
-          <t>01:44:00</t>
+          <t>00:59:25</t>
         </is>
       </c>
       <c r="H9" s="4" t="n">
-        <v>2.321</v>
+        <v>1.46</v>
       </c>
       <c r="I9" s="4" t="n">
-        <v>0.7137122732006727</v>
+        <v>0.2824090407989382</v>
       </c>
       <c r="J9" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-107280605- -APNSDYME# ENACOM</t>
+          <t>EX-2025-107254049- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K9" s="4" t="inlineStr">
@@ -686,32 +686,32 @@
       </c>
       <c r="C10" s="4" t="inlineStr">
         <is>
-          <t>Gobernador Costa</t>
+          <t>Dique F. Ameghino</t>
         </is>
       </c>
       <c r="D10" s="5" t="n">
-        <v>45789.62898148148</v>
+        <v>45874.53252314815</v>
       </c>
       <c r="E10" s="5" t="n">
-        <v>45789.67918981481</v>
+        <v>45874.56041666667</v>
       </c>
       <c r="F10" s="4" t="n">
-        <v>759</v>
+        <v>230</v>
       </c>
       <c r="G10" s="4" t="inlineStr">
         <is>
-          <t>01:12:18</t>
+          <t>00:40:10</t>
         </is>
       </c>
       <c r="H10" s="4" t="n">
-        <v>2.899</v>
+        <v>2.73</v>
       </c>
       <c r="I10" s="4" t="n">
-        <v>1.11344639852293</v>
+        <v>0.9874114937935857</v>
       </c>
       <c r="J10" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-51927249-APN- - SDYME#ENACOM</t>
+          <t>EX-2025-86907217- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K10" s="4" t="inlineStr">
@@ -733,32 +733,32 @@
       </c>
       <c r="C11" s="4" t="inlineStr">
         <is>
-          <t>Jose de San Martín</t>
+          <t>Dolavon</t>
         </is>
       </c>
       <c r="D11" s="5" t="n">
-        <v>45790.40565972222</v>
+        <v>45875.47517361111</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>45790.45607638889</v>
+        <v>45875.54798611111</v>
       </c>
       <c r="F11" s="4" t="n">
-        <v>770</v>
+        <v>950</v>
       </c>
       <c r="G11" s="4" t="inlineStr">
         <is>
-          <t>01:12:36</t>
+          <t>01:40:27</t>
         </is>
       </c>
       <c r="H11" s="4" t="n">
-        <v>1.863</v>
+        <v>2.987</v>
       </c>
       <c r="I11" s="4" t="n">
-        <v>0.4598313680449851</v>
+        <v>1.182070364578731</v>
       </c>
       <c r="J11" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-51925383-APN- - SDYME#ENACOM</t>
+          <t>EX-2025-86907862- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K11" s="4" t="inlineStr">
@@ -780,37 +780,37 @@
       </c>
       <c r="C12" s="4" t="inlineStr">
         <is>
-          <t>Puerto Madryn</t>
+          <t>El Hoyo</t>
         </is>
       </c>
       <c r="D12" s="5" t="n">
-        <v>45817.59449074074</v>
+        <v>45923.65008101852</v>
       </c>
       <c r="E12" s="5" t="n">
-        <v>45821.42857638889</v>
+        <v>45923.71108796296</v>
       </c>
       <c r="F12" s="4" t="n">
-        <v>10175</v>
+        <v>917</v>
       </c>
       <c r="G12" s="4" t="inlineStr">
         <is>
-          <t>17:03:07</t>
+          <t>01:27:51</t>
         </is>
       </c>
       <c r="H12" s="4" t="n">
-        <v>10.744</v>
+        <v>5.38</v>
       </c>
       <c r="I12" s="4" t="n">
-        <v>15.29342943225263</v>
+        <v>3.834753349831483</v>
       </c>
       <c r="J12" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-65041629-APN- - SDYME#ENACOM</t>
+          <t>EX-2025-107270163- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K12" s="4" t="inlineStr">
         <is>
-          <t>EF1891</t>
+          <t>EF0391</t>
         </is>
       </c>
     </row>
@@ -827,32 +827,32 @@
       </c>
       <c r="C13" s="4" t="inlineStr">
         <is>
-          <t>Rada Tilly</t>
+          <t>El Maiten</t>
         </is>
       </c>
       <c r="D13" s="5" t="n">
-        <v>45786.41888888889</v>
+        <v>45924.47306712963</v>
       </c>
       <c r="E13" s="5" t="n">
-        <v>45805.66069444444</v>
+        <v>45924.54931712963</v>
       </c>
       <c r="F13" s="4" t="n">
-        <v>2878</v>
+        <v>1042</v>
       </c>
       <c r="G13" s="4" t="inlineStr">
         <is>
-          <t>06:51:55</t>
+          <t>01:44:00</t>
         </is>
       </c>
       <c r="H13" s="4" t="n">
-        <v>3.21</v>
+        <v>2.321</v>
       </c>
       <c r="I13" s="4" t="n">
-        <v>1.365158095935607</v>
+        <v>0.7137122732006727</v>
       </c>
       <c r="J13" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-57494683-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-107280605- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K13" s="4" t="inlineStr">
@@ -874,37 +874,37 @@
       </c>
       <c r="C14" s="4" t="inlineStr">
         <is>
-          <t>Rawson</t>
+          <t>Epuyen</t>
         </is>
       </c>
       <c r="D14" s="5" t="n">
-        <v>45852.5327662037</v>
+        <v>45923.54929398148</v>
       </c>
       <c r="E14" s="5" t="n">
-        <v>45854.55157407407</v>
+        <v>45923.60721064815</v>
       </c>
       <c r="F14" s="4" t="n">
-        <v>5438</v>
+        <v>946</v>
       </c>
       <c r="G14" s="4" t="inlineStr">
         <is>
-          <t>08:22:28</t>
+          <t>01:23:24</t>
         </is>
       </c>
       <c r="H14" s="4" t="n">
-        <v>10.067</v>
+        <v>3.425</v>
       </c>
       <c r="I14" s="4" t="n">
-        <v>13.42681550419805</v>
+        <v>1.554153947373825</v>
       </c>
       <c r="J14" s="4" t="inlineStr">
         <is>
-          <t>EX-2025- 78894383- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-107283514- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K14" s="4" t="inlineStr">
         <is>
-          <t>EF1891</t>
+          <t>EF0391</t>
         </is>
       </c>
     </row>
@@ -921,32 +921,32 @@
       </c>
       <c r="C15" s="4" t="inlineStr">
         <is>
-          <t>Río Mayo</t>
+          <t>Gaiman</t>
         </is>
       </c>
       <c r="D15" s="5" t="n">
-        <v>45791.45833333334</v>
+        <v>45875.61319444444</v>
       </c>
       <c r="E15" s="5" t="n">
-        <v>45791.50844907408</v>
+        <v>45876.43600694444</v>
       </c>
       <c r="F15" s="4" t="n">
-        <v>852</v>
+        <v>1147</v>
       </c>
       <c r="G15" s="4" t="inlineStr">
         <is>
-          <t>01:12:10</t>
+          <t>02:07:24</t>
         </is>
       </c>
       <c r="H15" s="4" t="n">
-        <v>8.367000000000001</v>
+        <v>3.325</v>
       </c>
       <c r="I15" s="4" t="n">
-        <v>9.27496804747588</v>
+        <v>1.464725301033385</v>
       </c>
       <c r="J15" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-51927482-APN- - SDYME#ENACOM</t>
+          <t>EX-2025-86907684- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K15" s="4" t="inlineStr">
@@ -968,32 +968,32 @@
       </c>
       <c r="C16" s="4" t="inlineStr">
         <is>
-          <t>Río Pico</t>
+          <t>Gobernador Costa</t>
         </is>
       </c>
       <c r="D16" s="5" t="n">
-        <v>45790.61751157408</v>
+        <v>45789.62898148148</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>45790.66715277778</v>
+        <v>45789.67918981481</v>
       </c>
       <c r="F16" s="4" t="n">
-        <v>684</v>
+        <v>759</v>
       </c>
       <c r="G16" s="4" t="inlineStr">
         <is>
-          <t>01:11:29</t>
+          <t>01:12:18</t>
         </is>
       </c>
       <c r="H16" s="4" t="n">
-        <v>1.843</v>
+        <v>2.899</v>
       </c>
       <c r="I16" s="4" t="n">
-        <v>0.4500114402423874</v>
+        <v>1.11344639852293</v>
       </c>
       <c r="J16" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-51931624-APN- - SDYME#ENACOM</t>
+          <t>EX-2025-51927249-APN- - SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K16" s="4" t="inlineStr">
@@ -1015,32 +1015,32 @@
       </c>
       <c r="C17" s="4" t="inlineStr">
         <is>
-          <t>Sarmiento</t>
+          <t>Jose de San Martín</t>
         </is>
       </c>
       <c r="D17" s="5" t="n">
-        <v>45791.65675925926</v>
+        <v>45790.40565972222</v>
       </c>
       <c r="E17" s="5" t="n">
-        <v>45792.49758101852</v>
+        <v>45790.45607638889</v>
       </c>
       <c r="F17" s="4" t="n">
-        <v>2499</v>
+        <v>770</v>
       </c>
       <c r="G17" s="4" t="inlineStr">
         <is>
-          <t>04:10:03</t>
+          <t>01:12:36</t>
         </is>
       </c>
       <c r="H17" s="4" t="n">
-        <v>5.587</v>
+        <v>1.863</v>
       </c>
       <c r="I17" s="4" t="n">
-        <v>4.135520965585604</v>
+        <v>0.4598313680449851</v>
       </c>
       <c r="J17" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-51931433-APN- - SDYME#ENACOM</t>
+          <t>EX-2025-51925383-APN- - SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K17" s="4" t="inlineStr">
@@ -1062,37 +1062,37 @@
       </c>
       <c r="C18" s="4" t="inlineStr">
         <is>
-          <t>Trelew</t>
+          <t>Lago Puelo</t>
         </is>
       </c>
       <c r="D18" s="5" t="n">
-        <v>45854.63928240741</v>
+        <v>45924.61511574074</v>
       </c>
       <c r="E18" s="5" t="n">
-        <v>45856.53826388889</v>
+        <v>45924.70357638889</v>
       </c>
       <c r="F18" s="4" t="n">
-        <v>8067</v>
+        <v>1208</v>
       </c>
       <c r="G18" s="4" t="inlineStr">
         <is>
-          <t>12:46:48</t>
+          <t>02:03:18</t>
         </is>
       </c>
       <c r="H18" s="4" t="n">
-        <v>10.925</v>
+        <v>2.439</v>
       </c>
       <c r="I18" s="4" t="n">
-        <v>15.81305478054409</v>
+        <v>0.7881275059065965</v>
       </c>
       <c r="J18" s="4" t="inlineStr">
         <is>
-          <t>EX- 2025-78894044- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-107271922- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K18" s="4" t="inlineStr">
         <is>
-          <t>EF1891</t>
+          <t>EF0391</t>
         </is>
       </c>
     </row>
@@ -1104,37 +1104,37 @@
       </c>
       <c r="B19" s="4" t="inlineStr">
         <is>
-          <t>Santa Cruz</t>
+          <t>Chubut</t>
         </is>
       </c>
       <c r="C19" s="4" t="inlineStr">
         <is>
-          <t>28 de Noviembre</t>
+          <t>Las Plumas</t>
         </is>
       </c>
       <c r="D19" s="5" t="n">
-        <v>45722.52990740741</v>
+        <v>45874.46862268518</v>
       </c>
       <c r="E19" s="5" t="n">
-        <v>45722.77141203704</v>
+        <v>45874.4915625</v>
       </c>
       <c r="F19" s="4" t="n">
-        <v>1328</v>
+        <v>300</v>
       </c>
       <c r="G19" s="4" t="inlineStr">
         <is>
-          <t>03:12:59</t>
+          <t>00:33:02</t>
         </is>
       </c>
       <c r="H19" s="4" t="n">
-        <v>3.459</v>
+        <v>2.929</v>
       </c>
       <c r="I19" s="4" t="n">
-        <v>1.585163297370652</v>
+        <v>1.136610405228356</v>
       </c>
       <c r="J19" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-26350283- -APNSDYME# ENACOM</t>
+          <t>EX-2025-86907028 - -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K19" s="4" t="inlineStr">
@@ -1151,42 +1151,42 @@
       </c>
       <c r="B20" s="4" t="inlineStr">
         <is>
-          <t>Santa Cruz</t>
+          <t>Chubut</t>
         </is>
       </c>
       <c r="C20" s="4" t="inlineStr">
         <is>
-          <t>Cañadon Seco</t>
+          <t>Puerto Madryn</t>
         </is>
       </c>
       <c r="D20" s="5" t="n">
-        <v>45772.44009259259</v>
+        <v>45817.59449074074</v>
       </c>
       <c r="E20" s="5" t="n">
-        <v>45772.48277777778</v>
+        <v>45821.42857638889</v>
       </c>
       <c r="F20" s="4" t="n">
-        <v>566</v>
+        <v>10175</v>
       </c>
       <c r="G20" s="4" t="inlineStr">
         <is>
-          <t>01:01:28</t>
+          <t>17:03:07</t>
         </is>
       </c>
       <c r="H20" s="4" t="n">
-        <v>0.848</v>
+        <v>10.744</v>
       </c>
       <c r="I20" s="4" t="n">
-        <v>0.09527184784888333</v>
+        <v>15.29342943225263</v>
       </c>
       <c r="J20" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-44885465- -APNSDYME# ENACOM</t>
+          <t>EX-2025-65041629-APN- - SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K20" s="4" t="inlineStr">
         <is>
-          <t>EF0391</t>
+          <t>EF1891</t>
         </is>
       </c>
     </row>
@@ -1198,37 +1198,37 @@
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>Santa Cruz</t>
+          <t>Chubut</t>
         </is>
       </c>
       <c r="C21" s="4" t="inlineStr">
         <is>
-          <t>El Calafate</t>
+          <t>Puerto Piramides</t>
         </is>
       </c>
       <c r="D21" s="5" t="n">
-        <v>45725.38012731481</v>
+        <v>45818.44252314815</v>
       </c>
       <c r="E21" s="5" t="n">
-        <v>45725.89113425926</v>
+        <v>45818.46755787037</v>
       </c>
       <c r="F21" s="4" t="n">
-        <v>5098</v>
+        <v>235</v>
       </c>
       <c r="G21" s="4" t="inlineStr">
         <is>
-          <t>08:31:23</t>
+          <t>00:36:03</t>
         </is>
       </c>
       <c r="H21" s="4" t="n">
-        <v>5.991</v>
+        <v>0.795</v>
       </c>
       <c r="I21" s="4" t="n">
-        <v>4.755229952846593</v>
+        <v>0.08373502252343262</v>
       </c>
       <c r="J21" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-26350807- -APNSDYME# ENACOM</t>
+          <t>EX-2025-65042089-APN- - SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K21" s="4" t="inlineStr">
@@ -1245,37 +1245,37 @@
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
-          <t>Santa Cruz</t>
+          <t>Chubut</t>
         </is>
       </c>
       <c r="C22" s="4" t="inlineStr">
         <is>
-          <t>El Chalten</t>
+          <t>Rada Tilly</t>
         </is>
       </c>
       <c r="D22" s="5" t="n">
-        <v>45724.53105324074</v>
+        <v>45786.41888888889</v>
       </c>
       <c r="E22" s="5" t="n">
-        <v>45724.5831712963</v>
+        <v>45805.66069444444</v>
       </c>
       <c r="F22" s="4" t="n">
-        <v>458</v>
+        <v>2878</v>
       </c>
       <c r="G22" s="4" t="inlineStr">
         <is>
-          <t>01:15:03</t>
+          <t>06:51:55</t>
         </is>
       </c>
       <c r="H22" s="4" t="n">
-        <v>5.076</v>
+        <v>3.21</v>
       </c>
       <c r="I22" s="4" t="n">
-        <v>3.413627362357058</v>
+        <v>1.365158095935607</v>
       </c>
       <c r="J22" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-26350683- -APNSDYME# ENACOM</t>
+          <t>EX-2025-57494683-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K22" s="4" t="inlineStr">
@@ -1292,42 +1292,42 @@
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>Santa Cruz</t>
+          <t>Chubut</t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
         <is>
-          <t>Fitz Roy</t>
+          <t>Rawson</t>
         </is>
       </c>
       <c r="D23" s="5" t="n">
-        <v>45777.47289351852</v>
+        <v>45852.5327662037</v>
       </c>
       <c r="E23" s="5" t="n">
-        <v>45777.50890046296</v>
+        <v>45854.55157407407</v>
       </c>
       <c r="F23" s="4" t="n">
-        <v>442</v>
+        <v>5438</v>
       </c>
       <c r="G23" s="4" t="inlineStr">
         <is>
-          <t>00:51:51</t>
+          <t>08:22:28</t>
         </is>
       </c>
       <c r="H23" s="4" t="n">
-        <v>1.221</v>
+        <v>10.067</v>
       </c>
       <c r="I23" s="4" t="n">
-        <v>0.1975168778353022</v>
+        <v>13.42681550419805</v>
       </c>
       <c r="J23" s="4" t="inlineStr">
         <is>
-          <t>EX-2025- 46399573- -APN-SDYME#ENACOM</t>
+          <t>EX-2025- 78894383- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K23" s="4" t="inlineStr">
         <is>
-          <t>EF0391</t>
+          <t>EF1891</t>
         </is>
       </c>
     </row>
@@ -1339,37 +1339,37 @@
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
-          <t>Santa Cruz</t>
+          <t>Chubut</t>
         </is>
       </c>
       <c r="C24" s="4" t="inlineStr">
         <is>
-          <t>Jaramillo</t>
+          <t>Río Mayo</t>
         </is>
       </c>
       <c r="D24" s="5" t="n">
-        <v>45775.47744212963</v>
+        <v>45791.45833333334</v>
       </c>
       <c r="E24" s="5" t="n">
-        <v>45775.49759259259</v>
+        <v>45791.50844907408</v>
       </c>
       <c r="F24" s="4" t="n">
-        <v>301</v>
+        <v>852</v>
       </c>
       <c r="G24" s="4" t="inlineStr">
         <is>
-          <t>00:29:01</t>
+          <t>01:12:10</t>
         </is>
       </c>
       <c r="H24" s="4" t="n">
-        <v>1.759</v>
+        <v>8.367000000000001</v>
       </c>
       <c r="I24" s="4" t="n">
-        <v>0.4099251488854474</v>
+        <v>9.27496804747588</v>
       </c>
       <c r="J24" s="4" t="inlineStr">
         <is>
-          <t>EX-2025- 46399813- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-51927482-APN- - SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K24" s="4" t="inlineStr">
@@ -1386,37 +1386,37 @@
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>Santa Cruz</t>
+          <t>Chubut</t>
         </is>
       </c>
       <c r="C25" s="4" t="inlineStr">
         <is>
-          <t>Koluel Kayke</t>
+          <t>Río Pico</t>
         </is>
       </c>
       <c r="D25" s="5" t="n">
-        <v>45770.76137731481</v>
+        <v>45790.61751157408</v>
       </c>
       <c r="E25" s="5" t="n">
-        <v>45770.7769212963</v>
+        <v>45790.66715277778</v>
       </c>
       <c r="F25" s="4" t="n">
-        <v>224</v>
+        <v>684</v>
       </c>
       <c r="G25" s="4" t="inlineStr">
         <is>
-          <t>00:22:23</t>
+          <t>01:11:29</t>
         </is>
       </c>
       <c r="H25" s="4" t="n">
-        <v>1.528</v>
+        <v>1.843</v>
       </c>
       <c r="I25" s="4" t="n">
-        <v>0.3093282557293622</v>
+        <v>0.4500114402423874</v>
       </c>
       <c r="J25" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-44888593- -APNSDYME# ENACOM</t>
+          <t>EX-2025-51931624-APN- - SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K25" s="4" t="inlineStr">
@@ -1433,37 +1433,37 @@
       </c>
       <c r="B26" s="4" t="inlineStr">
         <is>
-          <t>Santa Cruz</t>
+          <t>Chubut</t>
         </is>
       </c>
       <c r="C26" s="4" t="inlineStr">
         <is>
-          <t>Las Heras</t>
+          <t>Sarmiento</t>
         </is>
       </c>
       <c r="D26" s="5" t="n">
-        <v>45769.6825925926</v>
+        <v>45791.65675925926</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>45770.69950231481</v>
+        <v>45792.49758101852</v>
       </c>
       <c r="F26" s="4" t="n">
-        <v>3469</v>
+        <v>2499</v>
       </c>
       <c r="G26" s="4" t="inlineStr">
         <is>
-          <t>06:13:06</t>
+          <t>04:10:03</t>
         </is>
       </c>
       <c r="H26" s="4" t="n">
-        <v>4.318</v>
+        <v>5.587</v>
       </c>
       <c r="I26" s="4" t="n">
-        <v>2.470234370621722</v>
+        <v>4.135520965585604</v>
       </c>
       <c r="J26" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-44888902- -APNSDYME# ENACOM</t>
+          <t>EX-2025-51931433-APN- - SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K26" s="4" t="inlineStr">
@@ -1480,42 +1480,42 @@
       </c>
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t>Santa Cruz</t>
+          <t>Chubut</t>
         </is>
       </c>
       <c r="C27" s="4" t="inlineStr">
         <is>
-          <t>Los Antiguos</t>
+          <t>Trelew</t>
         </is>
       </c>
       <c r="D27" s="5" t="n">
-        <v>45769.42946759259</v>
+        <v>45854.63928240741</v>
       </c>
       <c r="E27" s="5" t="n">
-        <v>45769.51760416666</v>
+        <v>45856.53826388889</v>
       </c>
       <c r="F27" s="4" t="n">
-        <v>1085</v>
+        <v>8067</v>
       </c>
       <c r="G27" s="4" t="inlineStr">
         <is>
-          <t>02:02:41</t>
+          <t>12:46:48</t>
         </is>
       </c>
       <c r="H27" s="4" t="n">
-        <v>2.739</v>
+        <v>10.925</v>
       </c>
       <c r="I27" s="4" t="n">
-        <v>0.9939326306847305</v>
+        <v>15.81305478054409</v>
       </c>
       <c r="J27" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-44890916- -APNSDYME# ENACOM</t>
+          <t>EX- 2025-78894044- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K27" s="4" t="inlineStr">
         <is>
-          <t>EF0391</t>
+          <t>EF1891</t>
         </is>
       </c>
     </row>
@@ -1532,32 +1532,32 @@
       </c>
       <c r="C28" s="4" t="inlineStr">
         <is>
-          <t>Perito Moreno</t>
+          <t>28 de Noviembre</t>
         </is>
       </c>
       <c r="D28" s="5" t="n">
-        <v>45768.63813657407</v>
+        <v>45722.52990740741</v>
       </c>
       <c r="E28" s="5" t="n">
-        <v>45768.7884837963</v>
+        <v>45722.77141203704</v>
       </c>
       <c r="F28" s="4" t="n">
-        <v>1350</v>
+        <v>1328</v>
       </c>
       <c r="G28" s="4" t="inlineStr">
         <is>
-          <t>02:53:22</t>
+          <t>03:12:59</t>
         </is>
       </c>
       <c r="H28" s="4" t="n">
-        <v>11.549</v>
+        <v>3.459</v>
       </c>
       <c r="I28" s="4" t="n">
-        <v>17.67102115722788</v>
+        <v>1.585163297370652</v>
       </c>
       <c r="J28" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-44890944- -APNSDYME# ENACOM</t>
+          <t>EX-2025-26350283- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K28" s="4" t="inlineStr">
@@ -1579,32 +1579,32 @@
       </c>
       <c r="C29" s="4" t="inlineStr">
         <is>
-          <t>Pico Truncado</t>
+          <t>Cañadon Seco</t>
         </is>
       </c>
       <c r="D29" s="5" t="n">
-        <v>45771.40826388889</v>
+        <v>45772.44009259259</v>
       </c>
       <c r="E29" s="5" t="n">
-        <v>45772.41405092592</v>
+        <v>45772.48277777778</v>
       </c>
       <c r="F29" s="4" t="n">
-        <v>3662</v>
+        <v>566</v>
       </c>
       <c r="G29" s="4" t="inlineStr">
         <is>
-          <t>06:27:50</t>
+          <t>01:01:28</t>
         </is>
       </c>
       <c r="H29" s="4" t="n">
-        <v>11.692</v>
+        <v>0.848</v>
       </c>
       <c r="I29" s="4" t="n">
-        <v>18.11133641241683</v>
+        <v>0.09527184784888333</v>
       </c>
       <c r="J29" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-44900833- -APNSDYME# ENACOM</t>
+          <t>EX-2025-44885465- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K29" s="4" t="inlineStr">
@@ -1626,32 +1626,32 @@
       </c>
       <c r="C30" s="4" t="inlineStr">
         <is>
-          <t>Puerto Deseado</t>
+          <t>Comandante Luis Pidrabuena</t>
         </is>
       </c>
       <c r="D30" s="5" t="n">
-        <v>45775.63364583333</v>
+        <v>45930.6691087963</v>
       </c>
       <c r="E30" s="5" t="n">
-        <v>45776.65954861111</v>
+        <v>45931.46759259259</v>
       </c>
       <c r="F30" s="4" t="n">
-        <v>2551</v>
+        <v>1651</v>
       </c>
       <c r="G30" s="4" t="inlineStr">
         <is>
-          <t>05:07:21</t>
+          <t>02:14:34</t>
         </is>
       </c>
       <c r="H30" s="4" t="n">
-        <v>8.297000000000001</v>
+        <v>7.273</v>
       </c>
       <c r="I30" s="4" t="n">
-        <v>9.120424747648924</v>
+        <v>7.008096273448687</v>
       </c>
       <c r="J30" s="4" t="inlineStr">
         <is>
-          <t>EX-2025- 46399962- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-110372903- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K30" s="4" t="inlineStr">
@@ -1673,37 +1673,37 @@
       </c>
       <c r="C31" s="4" t="inlineStr">
         <is>
-          <t>Rio Gallegos</t>
+          <t>El Calafate</t>
         </is>
       </c>
       <c r="D31" s="5" t="n">
-        <v>45734.37574074074</v>
+        <v>45725.38012731481</v>
       </c>
       <c r="E31" s="5" t="n">
-        <v>45736.7022337963</v>
+        <v>45725.89113425926</v>
       </c>
       <c r="F31" s="4" t="n">
-        <v>10546</v>
+        <v>5098</v>
       </c>
       <c r="G31" s="4" t="inlineStr">
         <is>
-          <t>17:49:33</t>
+          <t>08:31:23</t>
         </is>
       </c>
       <c r="H31" s="4" t="n">
-        <v>12.385</v>
+        <v>5.991</v>
       </c>
       <c r="I31" s="4" t="n">
-        <v>20.32192789083399</v>
+        <v>4.755229952846593</v>
       </c>
       <c r="J31" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-30586509- -APNSDYME# ENACOM</t>
+          <t>EX-2025-26350807- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K31" s="4" t="inlineStr">
         <is>
-          <t>EF1891</t>
+          <t>EF0391</t>
         </is>
       </c>
     </row>
@@ -1720,32 +1720,32 @@
       </c>
       <c r="C32" s="4" t="inlineStr">
         <is>
-          <t>Río Turbio</t>
+          <t>El Chalten</t>
         </is>
       </c>
       <c r="D32" s="5" t="n">
-        <v>45722.77626157407</v>
+        <v>45724.53105324074</v>
       </c>
       <c r="E32" s="5" t="n">
-        <v>45723.54744212963</v>
+        <v>45724.5831712963</v>
       </c>
       <c r="F32" s="4" t="n">
-        <v>1596</v>
+        <v>458</v>
       </c>
       <c r="G32" s="4" t="inlineStr">
         <is>
-          <t>03:40:52</t>
+          <t>01:15:03</t>
         </is>
       </c>
       <c r="H32" s="4" t="n">
-        <v>10.208</v>
+        <v>5.076</v>
       </c>
       <c r="I32" s="4" t="n">
-        <v>13.80556569448233</v>
+        <v>3.413627362357058</v>
       </c>
       <c r="J32" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-26350560- -APNSDYME# ENACOM</t>
+          <t>EX-2025-26350683- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K32" s="4" t="inlineStr">
@@ -1757,42 +1757,42 @@
     <row r="33">
       <c r="A33" s="4" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Comodoro Rivadavia</t>
         </is>
       </c>
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Santa Cruz</t>
         </is>
       </c>
       <c r="C33" s="4" t="inlineStr">
         <is>
-          <t>Colonia Tirolesa</t>
+          <t>Fitz Roy</t>
         </is>
       </c>
       <c r="D33" s="5" t="n">
-        <v>45665.43331018519</v>
+        <v>45777.47289351852</v>
       </c>
       <c r="E33" s="5" t="n">
-        <v>45665.51574074074</v>
+        <v>45777.50890046296</v>
       </c>
       <c r="F33" s="4" t="n">
-        <v>1181</v>
+        <v>442</v>
       </c>
       <c r="G33" s="4" t="inlineStr">
         <is>
-          <t>01:58:42</t>
+          <t>00:51:51</t>
         </is>
       </c>
       <c r="H33" s="4" t="n">
-        <v>3.091</v>
+        <v>1.221</v>
       </c>
       <c r="I33" s="4" t="n">
-        <v>1.265816913461025</v>
+        <v>0.1975168778353022</v>
       </c>
       <c r="J33" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-02492718-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025- 46399573- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K33" s="4" t="inlineStr">
@@ -1804,42 +1804,42 @@
     <row r="34">
       <c r="A34" s="4" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Comodoro Rivadavia</t>
         </is>
       </c>
       <c r="B34" s="4" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Santa Cruz</t>
         </is>
       </c>
       <c r="C34" s="4" t="inlineStr">
         <is>
-          <t>Estación Colonia Tirolesa</t>
+          <t>Jaramillo</t>
         </is>
       </c>
       <c r="D34" s="5" t="n">
-        <v>45665.41315972222</v>
+        <v>45775.47744212963</v>
       </c>
       <c r="E34" s="5" t="n">
-        <v>45665.42842592593</v>
+        <v>45775.49759259259</v>
       </c>
       <c r="F34" s="4" t="n">
-        <v>224</v>
+        <v>301</v>
       </c>
       <c r="G34" s="4" t="inlineStr">
         <is>
-          <t>00:21:59</t>
+          <t>00:29:01</t>
         </is>
       </c>
       <c r="H34" s="4" t="n">
-        <v>4.109</v>
+        <v>1.759</v>
       </c>
       <c r="I34" s="4" t="n">
-        <v>2.23689277452309</v>
+        <v>0.4099251488854474</v>
       </c>
       <c r="J34" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-02492607-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025- 46399813- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K34" s="4" t="inlineStr">
@@ -1851,42 +1851,42 @@
     <row r="35">
       <c r="A35" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Comodoro Rivadavia</t>
         </is>
       </c>
       <c r="B35" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Santa Cruz</t>
         </is>
       </c>
       <c r="C35" s="4" t="inlineStr">
         <is>
-          <t>Centenario</t>
+          <t>Koluel Kayke</t>
         </is>
       </c>
       <c r="D35" s="5" t="n">
-        <v>45678.393125</v>
+        <v>45770.76137731481</v>
       </c>
       <c r="E35" s="5" t="n">
-        <v>45680.60211805555</v>
+        <v>45770.7769212963</v>
       </c>
       <c r="F35" s="4" t="n">
-        <v>8420</v>
+        <v>224</v>
       </c>
       <c r="G35" s="4" t="inlineStr">
         <is>
-          <t>12:06:48</t>
+          <t>00:22:23</t>
         </is>
       </c>
       <c r="H35" s="4" t="n">
-        <v>13.145</v>
+        <v>1.528</v>
       </c>
       <c r="I35" s="4" t="n">
-        <v>22.89254439337369</v>
+        <v>0.3093282557293622</v>
       </c>
       <c r="J35" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-09027358- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-44888593- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K35" s="4" t="inlineStr">
@@ -1898,42 +1898,42 @@
     <row r="36">
       <c r="A36" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Comodoro Rivadavia</t>
         </is>
       </c>
       <c r="B36" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Santa Cruz</t>
         </is>
       </c>
       <c r="C36" s="4" t="inlineStr">
         <is>
-          <t>Chos Malal</t>
+          <t>Las Heras</t>
         </is>
       </c>
       <c r="D36" s="5" t="n">
-        <v>45699.39045138889</v>
+        <v>45769.6825925926</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>45699.55277777778</v>
+        <v>45770.69950231481</v>
       </c>
       <c r="F36" s="4" t="n">
-        <v>2767</v>
+        <v>3469</v>
       </c>
       <c r="G36" s="4" t="inlineStr">
         <is>
-          <t>03:53:45</t>
+          <t>06:13:06</t>
         </is>
       </c>
       <c r="H36" s="4" t="n">
-        <v>5.844</v>
+        <v>4.318</v>
       </c>
       <c r="I36" s="4" t="n">
-        <v>4.524736559768742</v>
+        <v>2.470234370621722</v>
       </c>
       <c r="J36" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-20181898- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-44888902- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K36" s="4" t="inlineStr">
@@ -1945,42 +1945,42 @@
     <row r="37">
       <c r="A37" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Comodoro Rivadavia</t>
         </is>
       </c>
       <c r="B37" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Santa Cruz</t>
         </is>
       </c>
       <c r="C37" s="4" t="inlineStr">
         <is>
-          <t>Las Lajas</t>
+          <t>Los Antiguos</t>
         </is>
       </c>
       <c r="D37" s="5" t="n">
-        <v>45700.44364583334</v>
+        <v>45769.42946759259</v>
       </c>
       <c r="E37" s="5" t="n">
-        <v>45700.53868055555</v>
+        <v>45769.51760416666</v>
       </c>
       <c r="F37" s="4" t="n">
-        <v>2144</v>
+        <v>1085</v>
       </c>
       <c r="G37" s="4" t="inlineStr">
         <is>
-          <t>02:16:51</t>
+          <t>02:02:41</t>
         </is>
       </c>
       <c r="H37" s="4" t="n">
-        <v>3.277</v>
+        <v>2.739</v>
       </c>
       <c r="I37" s="4" t="n">
-        <v>1.422740737610125</v>
+        <v>0.9939326306847305</v>
       </c>
       <c r="J37" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-20200350-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-44890916- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K37" s="4" t="inlineStr">
@@ -1992,42 +1992,42 @@
     <row r="38">
       <c r="A38" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Comodoro Rivadavia</t>
         </is>
       </c>
       <c r="B38" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Santa Cruz</t>
         </is>
       </c>
       <c r="C38" s="4" t="inlineStr">
         <is>
-          <t>Loncopue</t>
+          <t>Perito Moreno</t>
         </is>
       </c>
       <c r="D38" s="5" t="n">
-        <v>45698.57782407408</v>
+        <v>45768.63813657407</v>
       </c>
       <c r="E38" s="5" t="n">
-        <v>45698.67151620371</v>
+        <v>45768.7884837963</v>
       </c>
       <c r="F38" s="4" t="n">
-        <v>1400</v>
+        <v>1350</v>
       </c>
       <c r="G38" s="4" t="inlineStr">
         <is>
-          <t>02:14:55</t>
+          <t>02:53:22</t>
         </is>
       </c>
       <c r="H38" s="4" t="n">
-        <v>7.203</v>
+        <v>11.549</v>
       </c>
       <c r="I38" s="4" t="n">
-        <v>6.873844664693583</v>
+        <v>17.67102115722788</v>
       </c>
       <c r="J38" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-20278624-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-44890944- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K38" s="4" t="inlineStr">
@@ -2039,42 +2039,42 @@
     <row r="39">
       <c r="A39" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Comodoro Rivadavia</t>
         </is>
       </c>
       <c r="B39" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Santa Cruz</t>
         </is>
       </c>
       <c r="C39" s="4" t="inlineStr">
         <is>
-          <t>Plottier</t>
+          <t>Pico Truncado</t>
         </is>
       </c>
       <c r="D39" s="5" t="n">
-        <v>45692.46568287037</v>
+        <v>45771.40826388889</v>
       </c>
       <c r="E39" s="5" t="n">
-        <v>45695.57134259259</v>
+        <v>45772.41405092592</v>
       </c>
       <c r="F39" s="4" t="n">
-        <v>8602</v>
+        <v>3662</v>
       </c>
       <c r="G39" s="4" t="inlineStr">
         <is>
-          <t>13:05:56</t>
+          <t>06:27:50</t>
         </is>
       </c>
       <c r="H39" s="4" t="n">
-        <v>9.769</v>
+        <v>11.692</v>
       </c>
       <c r="I39" s="4" t="n">
-        <v>12.64366857770164</v>
+        <v>18.11133641241683</v>
       </c>
       <c r="J39" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-20278858-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-44900833- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K39" s="4" t="inlineStr">
@@ -2086,42 +2086,42 @@
     <row r="40">
       <c r="A40" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Comodoro Rivadavia</t>
         </is>
       </c>
       <c r="B40" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Santa Cruz</t>
         </is>
       </c>
       <c r="C40" s="4" t="inlineStr">
         <is>
-          <t>San Martín de los Andes</t>
+          <t>Puerto Deseado</t>
         </is>
       </c>
       <c r="D40" s="5" t="n">
-        <v>45756.63164351852</v>
+        <v>45775.63364583333</v>
       </c>
       <c r="E40" s="5" t="n">
-        <v>45757.56960648148</v>
+        <v>45776.65954861111</v>
       </c>
       <c r="F40" s="4" t="n">
-        <v>4021</v>
+        <v>2551</v>
       </c>
       <c r="G40" s="4" t="inlineStr">
         <is>
-          <t>06:04:59</t>
+          <t>05:07:21</t>
         </is>
       </c>
       <c r="H40" s="4" t="n">
-        <v>8.176</v>
+        <v>8.297000000000001</v>
       </c>
       <c r="I40" s="4" t="n">
-        <v>8.856347519454705</v>
+        <v>9.120424747648924</v>
       </c>
       <c r="J40" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-39977319- -APN-SDYME#ENACOM</t>
+          <t>EX-2025- 46399962- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K40" s="4" t="inlineStr">
@@ -2133,42 +2133,42 @@
     <row r="41">
       <c r="A41" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Comodoro Rivadavia</t>
         </is>
       </c>
       <c r="B41" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Santa Cruz</t>
         </is>
       </c>
       <c r="C41" s="4" t="inlineStr">
         <is>
-          <t>Senillosa</t>
+          <t>Puerto San Julián</t>
         </is>
       </c>
       <c r="D41" s="5" t="n">
-        <v>45741.4528125</v>
+        <v>45932.39018518518</v>
       </c>
       <c r="E41" s="5" t="n">
-        <v>45741.58811342593</v>
+        <v>45932.64784722222</v>
       </c>
       <c r="F41" s="4" t="n">
-        <v>2260</v>
+        <v>2280</v>
       </c>
       <c r="G41" s="4" t="inlineStr">
         <is>
-          <t>03:14:50</t>
+          <t>03:17:24</t>
         </is>
       </c>
       <c r="H41" s="4" t="n">
-        <v>6.355</v>
+        <v>13.727</v>
       </c>
       <c r="I41" s="4" t="n">
-        <v>5.350618587883253</v>
+        <v>24.96457353730838</v>
       </c>
       <c r="J41" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-32553095- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-110350271- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K41" s="4" t="inlineStr">
@@ -2180,42 +2180,42 @@
     <row r="42">
       <c r="A42" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Comodoro Rivadavia</t>
         </is>
       </c>
       <c r="B42" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Santa Cruz</t>
         </is>
       </c>
       <c r="C42" s="4" t="inlineStr">
         <is>
-          <t>Villa La Angostura</t>
+          <t>Puerto Santa Cruz</t>
         </is>
       </c>
       <c r="D42" s="5" t="n">
-        <v>45758.37885416667</v>
+        <v>45929.66099537037</v>
       </c>
       <c r="E42" s="5" t="n">
-        <v>45758.49877314815</v>
+        <v>45929.72302083333</v>
       </c>
       <c r="F42" s="4" t="n">
-        <v>2226</v>
+        <v>1127</v>
       </c>
       <c r="G42" s="4" t="inlineStr">
         <is>
-          <t>02:52:41</t>
+          <t>01:26:49</t>
         </is>
       </c>
       <c r="H42" s="4" t="n">
-        <v>6.26</v>
+        <v>2.599</v>
       </c>
       <c r="I42" s="4" t="n">
-        <v>5.19184299456393</v>
+        <v>0.8949225329319336</v>
       </c>
       <c r="J42" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-39977661- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-110372810- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K42" s="4" t="inlineStr">
@@ -2227,89 +2227,89 @@
     <row r="43">
       <c r="A43" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Comodoro Rivadavia</t>
         </is>
       </c>
       <c r="B43" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Santa Cruz</t>
         </is>
       </c>
       <c r="C43" s="4" t="inlineStr">
         <is>
-          <t>Zapala</t>
+          <t>Rio Gallegos</t>
         </is>
       </c>
       <c r="D43" s="5" t="n">
-        <v>45700.61767361111</v>
+        <v>45734.37574074074</v>
       </c>
       <c r="E43" s="5" t="n">
-        <v>45701.60255787037</v>
+        <v>45736.7022337963</v>
       </c>
       <c r="F43" s="4" t="n">
-        <v>5900</v>
+        <v>10546</v>
       </c>
       <c r="G43" s="4" t="inlineStr">
         <is>
-          <t>06:48:10</t>
+          <t>17:49:33</t>
         </is>
       </c>
       <c r="H43" s="4" t="n">
-        <v>7.476</v>
+        <v>12.385</v>
       </c>
       <c r="I43" s="4" t="n">
-        <v>7.404768229433365</v>
+        <v>20.32192789083399</v>
       </c>
       <c r="J43" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-20279172-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-30586509- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K43" s="4" t="inlineStr">
         <is>
-          <t>EF0391</t>
+          <t>EF1891</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="4" t="inlineStr">
         <is>
-          <t>Neuquén</t>
+          <t>Comodoro Rivadavia</t>
         </is>
       </c>
       <c r="B44" s="4" t="inlineStr">
         <is>
-          <t>Río Negro</t>
+          <t>Santa Cruz</t>
         </is>
       </c>
       <c r="C44" s="4" t="inlineStr">
         <is>
-          <t>Allen</t>
+          <t>Río Turbio</t>
         </is>
       </c>
       <c r="D44" s="5" t="n">
-        <v>45742.42247685185</v>
+        <v>45722.77626157407</v>
       </c>
       <c r="E44" s="5" t="n">
-        <v>45813.52212962963</v>
+        <v>45723.54744212963</v>
       </c>
       <c r="F44" s="4" t="n">
-        <v>5422</v>
+        <v>1596</v>
       </c>
       <c r="G44" s="4" t="inlineStr">
         <is>
-          <t>07:23:01</t>
+          <t>03:40:52</t>
         </is>
       </c>
       <c r="H44" s="4" t="n">
-        <v>10.342</v>
+        <v>10.208</v>
       </c>
       <c r="I44" s="4" t="n">
-        <v>14.17039482548629</v>
+        <v>13.80556569448233</v>
       </c>
       <c r="J44" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-62134249- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-26350560- -APNSDYME# ENACOM</t>
         </is>
       </c>
       <c r="K44" s="4" t="inlineStr">
@@ -2321,42 +2321,42 @@
     <row r="45">
       <c r="A45" s="4" t="inlineStr">
         <is>
-          <t>Posadas</t>
+          <t>Córdoba</t>
         </is>
       </c>
       <c r="B45" s="4" t="inlineStr">
         <is>
-          <t>Chaco</t>
+          <t>Córdoba</t>
         </is>
       </c>
       <c r="C45" s="4" t="inlineStr">
         <is>
-          <t>Barranqueras</t>
+          <t>Colonia Tirolesa</t>
         </is>
       </c>
       <c r="D45" s="5" t="n">
-        <v>45812.55844907407</v>
+        <v>45665.43331018519</v>
       </c>
       <c r="E45" s="5" t="n">
-        <v>45813.55945601852</v>
+        <v>45665.51574074074</v>
       </c>
       <c r="F45" s="4" t="n">
-        <v>1542</v>
+        <v>1181</v>
       </c>
       <c r="G45" s="4" t="inlineStr">
         <is>
-          <t>03:51:20</t>
+          <t>01:58:42</t>
         </is>
       </c>
       <c r="H45" s="4" t="n">
-        <v>11.927</v>
+        <v>3.091</v>
       </c>
       <c r="I45" s="4" t="n">
-        <v>18.84670022206126</v>
+        <v>1.265816913461025</v>
       </c>
       <c r="J45" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-97804852-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-02492718-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K45" s="4" t="inlineStr">
@@ -2368,42 +2368,42 @@
     <row r="46">
       <c r="A46" s="4" t="inlineStr">
         <is>
-          <t>Posadas</t>
+          <t>Córdoba</t>
         </is>
       </c>
       <c r="B46" s="4" t="inlineStr">
         <is>
-          <t>Chaco</t>
+          <t>Córdoba</t>
         </is>
       </c>
       <c r="C46" s="4" t="inlineStr">
         <is>
-          <t>Basail</t>
+          <t>Estación Colonia Tirolesa</t>
         </is>
       </c>
       <c r="D46" s="5" t="n">
-        <v>45916.46837962963</v>
+        <v>45665.41315972222</v>
       </c>
       <c r="E46" s="5" t="n">
-        <v>45916.5103125</v>
+        <v>45665.42842592593</v>
       </c>
       <c r="F46" s="4" t="n">
-        <v>811</v>
+        <v>224</v>
       </c>
       <c r="G46" s="4" t="inlineStr">
         <is>
-          <t>01:00:23</t>
+          <t>00:21:59</t>
         </is>
       </c>
       <c r="H46" s="4" t="n">
-        <v>8.038</v>
+        <v>4.109</v>
       </c>
       <c r="I46" s="4" t="n">
-        <v>8.559903878116309</v>
+        <v>2.23689277452309</v>
       </c>
       <c r="J46" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-105147378-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-02492607-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K46" s="4" t="inlineStr">
@@ -2415,42 +2415,42 @@
     <row r="47">
       <c r="A47" s="4" t="inlineStr">
         <is>
-          <t>Posadas</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="B47" s="4" t="inlineStr">
         <is>
-          <t>Chaco</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="C47" s="4" t="inlineStr">
         <is>
-          <t>Corzuela</t>
+          <t>Centenario</t>
         </is>
       </c>
       <c r="D47" s="5" t="n">
-        <v>45820.53369212963</v>
+        <v>45678.393125</v>
       </c>
       <c r="E47" s="5" t="n">
-        <v>45820.58216435185</v>
+        <v>45680.60211805555</v>
       </c>
       <c r="F47" s="4" t="n">
-        <v>799</v>
+        <v>8420</v>
       </c>
       <c r="G47" s="4" t="inlineStr">
         <is>
-          <t>01:09:48</t>
+          <t>12:06:48</t>
         </is>
       </c>
       <c r="H47" s="4" t="n">
-        <v>2.94</v>
+        <v>13.145</v>
       </c>
       <c r="I47" s="4" t="n">
-        <v>1.145163625938123</v>
+        <v>22.89254439337369</v>
       </c>
       <c r="J47" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73262047-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-09027358- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K47" s="4" t="inlineStr">
@@ -2462,42 +2462,42 @@
     <row r="48">
       <c r="A48" s="4" t="inlineStr">
         <is>
-          <t>Posadas</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="B48" s="4" t="inlineStr">
         <is>
-          <t>Chaco</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="C48" s="4" t="inlineStr">
         <is>
-          <t>Fontana</t>
+          <t>Chos Malal</t>
         </is>
       </c>
       <c r="D48" s="5" t="n">
-        <v>45918.52649305556</v>
+        <v>45699.39045138889</v>
       </c>
       <c r="E48" s="5" t="n">
-        <v>45918.56483796296</v>
+        <v>45699.55277777778</v>
       </c>
       <c r="F48" s="4" t="n">
-        <v>687</v>
+        <v>2767</v>
       </c>
       <c r="G48" s="4" t="inlineStr">
         <is>
-          <t>00:55:13</t>
+          <t>03:53:45</t>
         </is>
       </c>
       <c r="H48" s="4" t="n">
-        <v>6.305</v>
+        <v>5.844</v>
       </c>
       <c r="I48" s="4" t="n">
-        <v>5.26675439064844</v>
+        <v>4.524736559768742</v>
       </c>
       <c r="J48" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-105147260-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-20181898- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K48" s="4" t="inlineStr">
@@ -2509,42 +2509,42 @@
     <row r="49">
       <c r="A49" s="4" t="inlineStr">
         <is>
-          <t>Posadas</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="B49" s="4" t="inlineStr">
         <is>
-          <t>Chaco</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="C49" s="4" t="inlineStr">
         <is>
-          <t>General Pinedo</t>
+          <t>Las Lajas</t>
         </is>
       </c>
       <c r="D49" s="5" t="n">
-        <v>45820.41590277778</v>
+        <v>45700.44364583334</v>
       </c>
       <c r="E49" s="5" t="n">
-        <v>45820.45375</v>
+        <v>45700.53868055555</v>
       </c>
       <c r="F49" s="4" t="n">
-        <v>586</v>
+        <v>2144</v>
       </c>
       <c r="G49" s="4" t="inlineStr">
         <is>
-          <t>00:54:30</t>
+          <t>02:16:51</t>
         </is>
       </c>
       <c r="H49" s="4" t="n">
-        <v>5.347</v>
+        <v>3.277</v>
       </c>
       <c r="I49" s="4" t="n">
-        <v>3.787854185466004</v>
+        <v>1.422740737610125</v>
       </c>
       <c r="J49" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73254360-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-20200350-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K49" s="4" t="inlineStr">
@@ -2556,42 +2556,42 @@
     <row r="50">
       <c r="A50" s="4" t="inlineStr">
         <is>
-          <t>Posadas</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="B50" s="4" t="inlineStr">
         <is>
-          <t>Chaco</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="C50" s="4" t="inlineStr">
         <is>
-          <t>General San Martín</t>
+          <t>Loncopue</t>
         </is>
       </c>
       <c r="D50" s="5" t="n">
-        <v>45818.56168981481</v>
+        <v>45698.57782407408</v>
       </c>
       <c r="E50" s="5" t="n">
-        <v>45818.70513888889</v>
+        <v>45698.67151620371</v>
       </c>
       <c r="F50" s="4" t="n">
-        <v>914</v>
+        <v>1400</v>
       </c>
       <c r="G50" s="4" t="inlineStr">
         <is>
-          <t>01:35:41</t>
+          <t>02:14:55</t>
         </is>
       </c>
       <c r="H50" s="4" t="n">
-        <v>5.561</v>
+        <v>7.203</v>
       </c>
       <c r="I50" s="4" t="n">
-        <v>4.097119907386369</v>
+        <v>6.873844664693583</v>
       </c>
       <c r="J50" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73254137-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-20278624-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K50" s="4" t="inlineStr">
@@ -2603,42 +2603,42 @@
     <row r="51">
       <c r="A51" s="4" t="inlineStr">
         <is>
-          <t>Posadas</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="B51" s="4" t="inlineStr">
         <is>
-          <t>Chaco</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="C51" s="4" t="inlineStr">
         <is>
-          <t>Ituzaingo</t>
+          <t>Plottier</t>
         </is>
       </c>
       <c r="D51" s="5" t="n">
-        <v>45831.48724537037</v>
+        <v>45692.46568287037</v>
       </c>
       <c r="E51" s="5" t="n">
-        <v>45831.56583333333</v>
+        <v>45695.57134259259</v>
       </c>
       <c r="F51" s="4" t="n">
-        <v>1182</v>
+        <v>8602</v>
       </c>
       <c r="G51" s="4" t="inlineStr">
         <is>
-          <t>01:53:10</t>
+          <t>13:05:56</t>
         </is>
       </c>
       <c r="H51" s="4" t="n">
-        <v>9.388999999999999</v>
+        <v>9.769</v>
       </c>
       <c r="I51" s="4" t="n">
-        <v>11.67915876658421</v>
+        <v>12.64366857770164</v>
       </c>
       <c r="J51" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73252694-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-20278858-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K51" s="4" t="inlineStr">
@@ -2650,42 +2650,42 @@
     <row r="52">
       <c r="A52" s="4" t="inlineStr">
         <is>
-          <t>Posadas</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="B52" s="4" t="inlineStr">
         <is>
-          <t>Chaco</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="C52" s="4" t="inlineStr">
         <is>
-          <t>Las Breñas</t>
+          <t>San Martín de los Andes</t>
         </is>
       </c>
       <c r="D52" s="5" t="n">
-        <v>45819.71625</v>
+        <v>45756.63164351852</v>
       </c>
       <c r="E52" s="5" t="n">
-        <v>45819.76673611111</v>
+        <v>45757.56960648148</v>
       </c>
       <c r="F52" s="4" t="n">
-        <v>954</v>
+        <v>4021</v>
       </c>
       <c r="G52" s="4" t="inlineStr">
         <is>
-          <t>01:12:42</t>
+          <t>06:04:59</t>
         </is>
       </c>
       <c r="H52" s="4" t="n">
-        <v>3.477</v>
+        <v>8.176</v>
       </c>
       <c r="I52" s="4" t="n">
-        <v>1.60170401979778</v>
+        <v>8.856347519454705</v>
       </c>
       <c r="J52" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73253915-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-39977319- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K52" s="4" t="inlineStr">
@@ -2697,42 +2697,42 @@
     <row r="53">
       <c r="A53" s="4" t="inlineStr">
         <is>
-          <t>Posadas</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="B53" s="4" t="inlineStr">
         <is>
-          <t>Chaco</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="C53" s="4" t="inlineStr">
         <is>
-          <t>Machagai</t>
+          <t>Senillosa</t>
         </is>
       </c>
       <c r="D53" s="5" t="n">
-        <v>45819.50070601852</v>
+        <v>45741.4528125</v>
       </c>
       <c r="E53" s="5" t="n">
-        <v>45819.56872685185</v>
+        <v>45741.58811342593</v>
       </c>
       <c r="F53" s="4" t="n">
-        <v>794</v>
+        <v>2260</v>
       </c>
       <c r="G53" s="4" t="inlineStr">
         <is>
-          <t>01:37:57</t>
+          <t>03:14:50</t>
         </is>
       </c>
       <c r="H53" s="4" t="n">
-        <v>3.329</v>
+        <v>6.355</v>
       </c>
       <c r="I53" s="4" t="n">
-        <v>1.468251571923751</v>
+        <v>5.350618587883253</v>
       </c>
       <c r="J53" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73253720-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-32553095- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K53" s="4" t="inlineStr">
@@ -2744,42 +2744,42 @@
     <row r="54">
       <c r="A54" s="4" t="inlineStr">
         <is>
-          <t>Posadas</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="B54" s="4" t="inlineStr">
         <is>
-          <t>Chaco</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="C54" s="4" t="inlineStr">
         <is>
-          <t>Presidencia de la Plaza</t>
+          <t>Villa La Angostura</t>
         </is>
       </c>
       <c r="D54" s="5" t="n">
-        <v>45896.461875</v>
+        <v>45758.37885416667</v>
       </c>
       <c r="E54" s="5" t="n">
-        <v>45896.52564814815</v>
+        <v>45758.49877314815</v>
       </c>
       <c r="F54" s="4" t="n">
-        <v>865</v>
+        <v>2226</v>
       </c>
       <c r="G54" s="4" t="inlineStr">
         <is>
-          <t>01:31:50</t>
+          <t>02:52:41</t>
         </is>
       </c>
       <c r="H54" s="4" t="n">
-        <v>3.203</v>
+        <v>6.26</v>
       </c>
       <c r="I54" s="4" t="n">
-        <v>1.359210627249875</v>
+        <v>5.19184299456393</v>
       </c>
       <c r="J54" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-97797640-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-39977661- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K54" s="4" t="inlineStr">
@@ -2791,42 +2791,42 @@
     <row r="55">
       <c r="A55" s="4" t="inlineStr">
         <is>
-          <t>Posadas</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="B55" s="4" t="inlineStr">
         <is>
-          <t>Chaco</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="C55" s="4" t="inlineStr">
         <is>
-          <t>Puerto Vilelas</t>
+          <t>Zapala</t>
         </is>
       </c>
       <c r="D55" s="5" t="n">
-        <v>45812.42873842592</v>
+        <v>45700.61767361111</v>
       </c>
       <c r="E55" s="5" t="n">
-        <v>45812.53604166667</v>
+        <v>45701.60255787037</v>
       </c>
       <c r="F55" s="4" t="n">
-        <v>975</v>
+        <v>5900</v>
       </c>
       <c r="G55" s="4" t="inlineStr">
         <is>
-          <t>02:16:46</t>
+          <t>06:48:10</t>
         </is>
       </c>
       <c r="H55" s="4" t="n">
-        <v>13.864</v>
+        <v>7.476</v>
       </c>
       <c r="I55" s="4" t="n">
-        <v>25.46536958474769</v>
+        <v>7.404768229433365</v>
       </c>
       <c r="J55" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73253473-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-20279172-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K55" s="4" t="inlineStr">
@@ -2838,42 +2838,42 @@
     <row r="56">
       <c r="A56" s="4" t="inlineStr">
         <is>
-          <t>Posadas</t>
+          <t>Neuquén</t>
         </is>
       </c>
       <c r="B56" s="4" t="inlineStr">
         <is>
-          <t>Chaco</t>
+          <t>Río Negro</t>
         </is>
       </c>
       <c r="C56" s="4" t="inlineStr">
         <is>
-          <t>Quitipili</t>
+          <t>Allen</t>
         </is>
       </c>
       <c r="D56" s="5" t="n">
-        <v>45896.55892361111</v>
+        <v>45742.42247685185</v>
       </c>
       <c r="E56" s="5" t="n">
-        <v>45896.65435185185</v>
+        <v>45813.52212962963</v>
       </c>
       <c r="F56" s="4" t="n">
-        <v>1404</v>
+        <v>5422</v>
       </c>
       <c r="G56" s="4" t="inlineStr">
         <is>
-          <t>02:17:25</t>
+          <t>07:23:01</t>
         </is>
       </c>
       <c r="H56" s="4" t="n">
-        <v>3.1</v>
+        <v>10.342</v>
       </c>
       <c r="I56" s="4" t="n">
-        <v>1.273198950120941</v>
+        <v>14.17039482548629</v>
       </c>
       <c r="J56" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-97797814-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-62134249- -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K56" s="4" t="inlineStr">
@@ -2895,32 +2895,32 @@
       </c>
       <c r="C57" s="4" t="inlineStr">
         <is>
-          <t>Resistencia</t>
+          <t>Barranqueras</t>
         </is>
       </c>
       <c r="D57" s="5" t="n">
-        <v>45917.46174768519</v>
+        <v>45812.55844907407</v>
       </c>
       <c r="E57" s="5" t="n">
-        <v>45918.5246875</v>
+        <v>45813.55945601852</v>
       </c>
       <c r="F57" s="4" t="n">
-        <v>4525</v>
+        <v>1542</v>
       </c>
       <c r="G57" s="4" t="inlineStr">
         <is>
-          <t>07:29:04</t>
+          <t>03:51:20</t>
         </is>
       </c>
       <c r="H57" s="4" t="n">
-        <v>9.226000000000001</v>
+        <v>11.927</v>
       </c>
       <c r="I57" s="4" t="n">
-        <v>11.27716110285792</v>
+        <v>18.84670022206126</v>
       </c>
       <c r="J57" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-105147001-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-97804852-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K57" s="4" t="inlineStr">
@@ -2942,32 +2942,32 @@
       </c>
       <c r="C58" s="4" t="inlineStr">
         <is>
-          <t>Roque Saenz Peña</t>
+          <t>Basail</t>
         </is>
       </c>
       <c r="D58" s="5" t="n">
-        <v>45820.65457175926</v>
+        <v>45916.46837962963</v>
       </c>
       <c r="E58" s="5" t="n">
-        <v>45820.71850694445</v>
+        <v>45916.5103125</v>
       </c>
       <c r="F58" s="4" t="n">
-        <v>1139</v>
+        <v>811</v>
       </c>
       <c r="G58" s="4" t="inlineStr">
         <is>
-          <t>01:32:04</t>
+          <t>01:00:23</t>
         </is>
       </c>
       <c r="H58" s="4" t="n">
-        <v>4.777</v>
+        <v>8.038</v>
       </c>
       <c r="I58" s="4" t="n">
-        <v>3.023314776778812</v>
+        <v>8.559903878116309</v>
       </c>
       <c r="J58" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73253145-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-105147378-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K58" s="4" t="inlineStr">
@@ -2989,32 +2989,32 @@
       </c>
       <c r="C59" s="4" t="inlineStr">
         <is>
-          <t>Villa Ángela</t>
+          <t>Corzuela</t>
         </is>
       </c>
       <c r="D59" s="5" t="n">
-        <v>45897.51820601852</v>
+        <v>45820.53369212963</v>
       </c>
       <c r="E59" s="5" t="n">
-        <v>45897.66859953704</v>
+        <v>45820.58216435185</v>
       </c>
       <c r="F59" s="4" t="n">
-        <v>2380</v>
+        <v>799</v>
       </c>
       <c r="G59" s="4" t="inlineStr">
         <is>
-          <t>03:36:34</t>
+          <t>01:09:48</t>
         </is>
       </c>
       <c r="H59" s="4" t="n">
-        <v>7.56</v>
+        <v>2.94</v>
       </c>
       <c r="I59" s="4" t="n">
-        <v>7.572102342937794</v>
+        <v>1.145163625938123</v>
       </c>
       <c r="J59" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-97798907-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-73262047-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K59" s="4" t="inlineStr">
@@ -3031,37 +3031,37 @@
       </c>
       <c r="B60" s="4" t="inlineStr">
         <is>
-          <t>Corrientes</t>
+          <t>Chaco</t>
         </is>
       </c>
       <c r="C60" s="4" t="inlineStr">
         <is>
-          <t>Corrientes</t>
+          <t>Fontana</t>
         </is>
       </c>
       <c r="D60" s="5" t="n">
-        <v>45832.40711805555</v>
+        <v>45918.52649305556</v>
       </c>
       <c r="E60" s="5" t="n">
-        <v>45833.658125</v>
+        <v>45918.56483796296</v>
       </c>
       <c r="F60" s="4" t="n">
-        <v>7411</v>
+        <v>687</v>
       </c>
       <c r="G60" s="4" t="inlineStr">
         <is>
-          <t>12:49:16</t>
+          <t>00:55:13</t>
         </is>
       </c>
       <c r="H60" s="4" t="n">
-        <v>12.527</v>
+        <v>6.305</v>
       </c>
       <c r="I60" s="4" t="n">
-        <v>20.79060077104716</v>
+        <v>5.26675439064844</v>
       </c>
       <c r="J60" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73252918-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-105147260-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K60" s="4" t="inlineStr">
@@ -3078,37 +3078,37 @@
       </c>
       <c r="B61" s="4" t="inlineStr">
         <is>
-          <t>Corrientes</t>
+          <t>Chaco</t>
         </is>
       </c>
       <c r="C61" s="4" t="inlineStr">
         <is>
-          <t>Ituzaingo</t>
+          <t>General Pinedo</t>
         </is>
       </c>
       <c r="D61" s="5" t="n">
-        <v>45831.48724537037</v>
+        <v>45820.41590277778</v>
       </c>
       <c r="E61" s="5" t="n">
-        <v>45831.56583333333</v>
+        <v>45820.45375</v>
       </c>
       <c r="F61" s="4" t="n">
-        <v>1182</v>
+        <v>586</v>
       </c>
       <c r="G61" s="4" t="inlineStr">
         <is>
-          <t>01:53:10</t>
+          <t>00:54:30</t>
         </is>
       </c>
       <c r="H61" s="4" t="n">
-        <v>9.388999999999999</v>
+        <v>5.347</v>
       </c>
       <c r="I61" s="4" t="n">
-        <v>11.67915876658421</v>
+        <v>3.787854185466004</v>
       </c>
       <c r="J61" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73252694-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-73254360-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K61" s="4" t="inlineStr">
@@ -3125,37 +3125,37 @@
       </c>
       <c r="B62" s="4" t="inlineStr">
         <is>
-          <t>Corrientes</t>
+          <t>Chaco</t>
         </is>
       </c>
       <c r="C62" s="4" t="inlineStr">
         <is>
-          <t>Paso de la Patria</t>
+          <t>General San Martín</t>
         </is>
       </c>
       <c r="D62" s="5" t="n">
-        <v>45831.68550925926</v>
+        <v>45818.56168981481</v>
       </c>
       <c r="E62" s="5" t="n">
-        <v>45831.73684027778</v>
+        <v>45818.70513888889</v>
       </c>
       <c r="F62" s="4" t="n">
-        <v>828</v>
+        <v>914</v>
       </c>
       <c r="G62" s="4" t="inlineStr">
         <is>
-          <t>01:13:55</t>
+          <t>01:35:41</t>
         </is>
       </c>
       <c r="H62" s="4" t="n">
-        <v>3.111</v>
+        <v>5.561</v>
       </c>
       <c r="I62" s="4" t="n">
-        <v>1.282250586486312</v>
+        <v>4.097119907386369</v>
       </c>
       <c r="J62" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-73252434-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-73254137-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K62" s="4" t="inlineStr">
@@ -3172,37 +3172,37 @@
       </c>
       <c r="B63" s="4" t="inlineStr">
         <is>
-          <t>Formosa</t>
+          <t>Chaco</t>
         </is>
       </c>
       <c r="C63" s="4" t="inlineStr">
         <is>
-          <t>Formosa</t>
+          <t>Ituzaingo</t>
         </is>
       </c>
       <c r="D63" s="5" t="n">
-        <v>45847.47630787037</v>
+        <v>45831.48724537037</v>
       </c>
       <c r="E63" s="5" t="n">
-        <v>45848.71959490741</v>
+        <v>45831.56583333333</v>
       </c>
       <c r="F63" s="4" t="n">
-        <v>5553</v>
+        <v>1182</v>
       </c>
       <c r="G63" s="4" t="inlineStr">
         <is>
-          <t>10:32:42</t>
+          <t>01:53:10</t>
         </is>
       </c>
       <c r="H63" s="4" t="n">
-        <v>8.835000000000001</v>
+        <v>9.388999999999999</v>
       </c>
       <c r="I63" s="4" t="n">
-        <v>10.34155847235734</v>
+        <v>11.67915876658421</v>
       </c>
       <c r="J63" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-77142320-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-73252694-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K63" s="4" t="inlineStr">
@@ -3219,37 +3219,37 @@
       </c>
       <c r="B64" s="4" t="inlineStr">
         <is>
-          <t>Formosa</t>
+          <t>Chaco</t>
         </is>
       </c>
       <c r="C64" s="4" t="inlineStr">
         <is>
-          <t>Laguna Blanca</t>
+          <t>Las Breñas</t>
         </is>
       </c>
       <c r="D64" s="5" t="n">
-        <v>45846.4572337963</v>
+        <v>45819.71625</v>
       </c>
       <c r="E64" s="5" t="n">
-        <v>45846.50842592592</v>
+        <v>45819.76673611111</v>
       </c>
       <c r="F64" s="4" t="n">
-        <v>610</v>
+        <v>954</v>
       </c>
       <c r="G64" s="4" t="inlineStr">
         <is>
-          <t>01:13:43</t>
+          <t>01:12:42</t>
         </is>
       </c>
       <c r="H64" s="4" t="n">
-        <v>2.874</v>
+        <v>3.477</v>
       </c>
       <c r="I64" s="4" t="n">
-        <v>1.094325229066509</v>
+        <v>1.60170401979778</v>
       </c>
       <c r="J64" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-77142546-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-73253915-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K64" s="4" t="inlineStr">
@@ -3261,139 +3261,750 @@
     <row r="65">
       <c r="A65" s="4" t="inlineStr">
         <is>
-          <t>Salta</t>
+          <t>Posadas</t>
         </is>
       </c>
       <c r="B65" s="4" t="inlineStr">
         <is>
-          <t>Jujuy</t>
+          <t>Chaco</t>
         </is>
       </c>
       <c r="C65" s="4" t="inlineStr">
         <is>
-          <t>San Pablo de Reyes</t>
+          <t>Machagai</t>
         </is>
       </c>
       <c r="D65" s="5" t="n">
-        <v>45734.39631944444</v>
+        <v>45819.50070601852</v>
       </c>
       <c r="E65" s="5" t="n">
-        <v>45734.41811342593</v>
+        <v>45819.56872685185</v>
       </c>
       <c r="F65" s="4" t="n">
-        <v>260</v>
+        <v>794</v>
       </c>
       <c r="G65" s="4" t="inlineStr">
         <is>
-          <t>00:25:35</t>
+          <t>01:37:57</t>
         </is>
       </c>
       <c r="H65" s="4" t="n">
-        <v>4.246</v>
+        <v>3.329</v>
       </c>
       <c r="I65" s="4" t="n">
-        <v>2.388541898380706</v>
+        <v>1.468251571923751</v>
       </c>
       <c r="J65" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-33150525-   -APN-SDYME#ENACOM</t>
+          <t>EX-2025-73253720-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K65" s="4" t="inlineStr">
         <is>
-          <t>EF1891</t>
+          <t>EF0391</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="4" t="inlineStr">
         <is>
-          <t>Salta</t>
+          <t>Posadas</t>
         </is>
       </c>
       <c r="B66" s="4" t="inlineStr">
         <is>
-          <t>Jujuy</t>
+          <t>Chaco</t>
         </is>
       </c>
       <c r="C66" s="4" t="inlineStr">
         <is>
-          <t>San Salvador de Jujuy</t>
+          <t>Presidencia de la Plaza</t>
         </is>
       </c>
       <c r="D66" s="5" t="n">
-        <v>45734.45050925926</v>
+        <v>45896.461875</v>
       </c>
       <c r="E66" s="5" t="n">
-        <v>45736.80579861111</v>
+        <v>45896.52564814815</v>
       </c>
       <c r="F66" s="4" t="n">
-        <v>7808</v>
+        <v>865</v>
       </c>
       <c r="G66" s="4" t="inlineStr">
         <is>
-          <t>17:51:37</t>
+          <t>01:31:50</t>
         </is>
       </c>
       <c r="H66" s="4" t="n">
-        <v>16.837</v>
+        <v>3.203</v>
       </c>
       <c r="I66" s="4" t="n">
-        <v>37.55798705788629</v>
+        <v>1.359210627249875</v>
       </c>
       <c r="J66" s="4" t="inlineStr">
         <is>
-          <t>EX-2025-101525989- -APN-SDYME#ENACOM</t>
+          <t>EX-2025-97797640-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
       <c r="K66" s="4" t="inlineStr">
         <is>
-          <t>EF0391, EF1891</t>
+          <t>EF0391</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="4" t="inlineStr">
         <is>
+          <t>Posadas</t>
+        </is>
+      </c>
+      <c r="B67" s="4" t="inlineStr">
+        <is>
+          <t>Chaco</t>
+        </is>
+      </c>
+      <c r="C67" s="4" t="inlineStr">
+        <is>
+          <t>Puerto Vilelas</t>
+        </is>
+      </c>
+      <c r="D67" s="5" t="n">
+        <v>45812.42873842592</v>
+      </c>
+      <c r="E67" s="5" t="n">
+        <v>45812.53604166667</v>
+      </c>
+      <c r="F67" s="4" t="n">
+        <v>975</v>
+      </c>
+      <c r="G67" s="4" t="inlineStr">
+        <is>
+          <t>02:16:46</t>
+        </is>
+      </c>
+      <c r="H67" s="4" t="n">
+        <v>13.864</v>
+      </c>
+      <c r="I67" s="4" t="n">
+        <v>25.46536958474769</v>
+      </c>
+      <c r="J67" s="4" t="inlineStr">
+        <is>
+          <t>EX-2025-73253473-   -APN-SDYME#ENACOM</t>
+        </is>
+      </c>
+      <c r="K67" s="4" t="inlineStr">
+        <is>
+          <t>EF0391</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="4" t="inlineStr">
+        <is>
+          <t>Posadas</t>
+        </is>
+      </c>
+      <c r="B68" s="4" t="inlineStr">
+        <is>
+          <t>Chaco</t>
+        </is>
+      </c>
+      <c r="C68" s="4" t="inlineStr">
+        <is>
+          <t>Quitipili</t>
+        </is>
+      </c>
+      <c r="D68" s="5" t="n">
+        <v>45896.55892361111</v>
+      </c>
+      <c r="E68" s="5" t="n">
+        <v>45896.65435185185</v>
+      </c>
+      <c r="F68" s="4" t="n">
+        <v>1404</v>
+      </c>
+      <c r="G68" s="4" t="inlineStr">
+        <is>
+          <t>02:17:25</t>
+        </is>
+      </c>
+      <c r="H68" s="4" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="I68" s="4" t="n">
+        <v>1.273198950120941</v>
+      </c>
+      <c r="J68" s="4" t="inlineStr">
+        <is>
+          <t>EX-2025-97797814-   -APN-SDYME#ENACOM</t>
+        </is>
+      </c>
+      <c r="K68" s="4" t="inlineStr">
+        <is>
+          <t>EF0391</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="4" t="inlineStr">
+        <is>
+          <t>Posadas</t>
+        </is>
+      </c>
+      <c r="B69" s="4" t="inlineStr">
+        <is>
+          <t>Chaco</t>
+        </is>
+      </c>
+      <c r="C69" s="4" t="inlineStr">
+        <is>
+          <t>Resistencia</t>
+        </is>
+      </c>
+      <c r="D69" s="5" t="n">
+        <v>45917.46174768519</v>
+      </c>
+      <c r="E69" s="5" t="n">
+        <v>45918.5246875</v>
+      </c>
+      <c r="F69" s="4" t="n">
+        <v>4525</v>
+      </c>
+      <c r="G69" s="4" t="inlineStr">
+        <is>
+          <t>07:29:04</t>
+        </is>
+      </c>
+      <c r="H69" s="4" t="n">
+        <v>9.226000000000001</v>
+      </c>
+      <c r="I69" s="4" t="n">
+        <v>11.27716110285792</v>
+      </c>
+      <c r="J69" s="4" t="inlineStr">
+        <is>
+          <t>EX-2025-105147001-   -APN-SDYME#ENACOM</t>
+        </is>
+      </c>
+      <c r="K69" s="4" t="inlineStr">
+        <is>
+          <t>EF0391</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="4" t="inlineStr">
+        <is>
+          <t>Posadas</t>
+        </is>
+      </c>
+      <c r="B70" s="4" t="inlineStr">
+        <is>
+          <t>Chaco</t>
+        </is>
+      </c>
+      <c r="C70" s="4" t="inlineStr">
+        <is>
+          <t>Roque Saenz Peña</t>
+        </is>
+      </c>
+      <c r="D70" s="5" t="n">
+        <v>45820.65457175926</v>
+      </c>
+      <c r="E70" s="5" t="n">
+        <v>45820.71850694445</v>
+      </c>
+      <c r="F70" s="4" t="n">
+        <v>1139</v>
+      </c>
+      <c r="G70" s="4" t="inlineStr">
+        <is>
+          <t>01:32:04</t>
+        </is>
+      </c>
+      <c r="H70" s="4" t="n">
+        <v>4.777</v>
+      </c>
+      <c r="I70" s="4" t="n">
+        <v>3.023314776778812</v>
+      </c>
+      <c r="J70" s="4" t="inlineStr">
+        <is>
+          <t>EX-2025-73253145-   -APN-SDYME#ENACOM</t>
+        </is>
+      </c>
+      <c r="K70" s="4" t="inlineStr">
+        <is>
+          <t>EF0391</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="4" t="inlineStr">
+        <is>
+          <t>Posadas</t>
+        </is>
+      </c>
+      <c r="B71" s="4" t="inlineStr">
+        <is>
+          <t>Chaco</t>
+        </is>
+      </c>
+      <c r="C71" s="4" t="inlineStr">
+        <is>
+          <t>Villa Ángela</t>
+        </is>
+      </c>
+      <c r="D71" s="5" t="n">
+        <v>45897.51820601852</v>
+      </c>
+      <c r="E71" s="5" t="n">
+        <v>45897.66859953704</v>
+      </c>
+      <c r="F71" s="4" t="n">
+        <v>2380</v>
+      </c>
+      <c r="G71" s="4" t="inlineStr">
+        <is>
+          <t>03:36:34</t>
+        </is>
+      </c>
+      <c r="H71" s="4" t="n">
+        <v>7.56</v>
+      </c>
+      <c r="I71" s="4" t="n">
+        <v>7.572102342937794</v>
+      </c>
+      <c r="J71" s="4" t="inlineStr">
+        <is>
+          <t>EX-2025-97798907-   -APN-SDYME#ENACOM</t>
+        </is>
+      </c>
+      <c r="K71" s="4" t="inlineStr">
+        <is>
+          <t>EF0391</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="4" t="inlineStr">
+        <is>
+          <t>Posadas</t>
+        </is>
+      </c>
+      <c r="B72" s="4" t="inlineStr">
+        <is>
+          <t>Corrientes</t>
+        </is>
+      </c>
+      <c r="C72" s="4" t="inlineStr">
+        <is>
+          <t>Corrientes</t>
+        </is>
+      </c>
+      <c r="D72" s="5" t="n">
+        <v>45832.40711805555</v>
+      </c>
+      <c r="E72" s="5" t="n">
+        <v>45833.658125</v>
+      </c>
+      <c r="F72" s="4" t="n">
+        <v>7411</v>
+      </c>
+      <c r="G72" s="4" t="inlineStr">
+        <is>
+          <t>12:49:16</t>
+        </is>
+      </c>
+      <c r="H72" s="4" t="n">
+        <v>12.527</v>
+      </c>
+      <c r="I72" s="4" t="n">
+        <v>20.79060077104716</v>
+      </c>
+      <c r="J72" s="4" t="inlineStr">
+        <is>
+          <t>EX-2025-73252918-   -APN-SDYME#ENACOM</t>
+        </is>
+      </c>
+      <c r="K72" s="4" t="inlineStr">
+        <is>
+          <t>EF0391</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="4" t="inlineStr">
+        <is>
+          <t>Posadas</t>
+        </is>
+      </c>
+      <c r="B73" s="4" t="inlineStr">
+        <is>
+          <t>Corrientes</t>
+        </is>
+      </c>
+      <c r="C73" s="4" t="inlineStr">
+        <is>
+          <t>Ituzaingo</t>
+        </is>
+      </c>
+      <c r="D73" s="5" t="n">
+        <v>45831.48724537037</v>
+      </c>
+      <c r="E73" s="5" t="n">
+        <v>45831.56583333333</v>
+      </c>
+      <c r="F73" s="4" t="n">
+        <v>1182</v>
+      </c>
+      <c r="G73" s="4" t="inlineStr">
+        <is>
+          <t>01:53:10</t>
+        </is>
+      </c>
+      <c r="H73" s="4" t="n">
+        <v>9.388999999999999</v>
+      </c>
+      <c r="I73" s="4" t="n">
+        <v>11.67915876658421</v>
+      </c>
+      <c r="J73" s="4" t="inlineStr">
+        <is>
+          <t>EX-2025-73252694-   -APN-SDYME#ENACOM</t>
+        </is>
+      </c>
+      <c r="K73" s="4" t="inlineStr">
+        <is>
+          <t>EF0391</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="4" t="inlineStr">
+        <is>
+          <t>Posadas</t>
+        </is>
+      </c>
+      <c r="B74" s="4" t="inlineStr">
+        <is>
+          <t>Corrientes</t>
+        </is>
+      </c>
+      <c r="C74" s="4" t="inlineStr">
+        <is>
+          <t>Paso de la Patria</t>
+        </is>
+      </c>
+      <c r="D74" s="5" t="n">
+        <v>45831.68550925926</v>
+      </c>
+      <c r="E74" s="5" t="n">
+        <v>45831.73684027778</v>
+      </c>
+      <c r="F74" s="4" t="n">
+        <v>828</v>
+      </c>
+      <c r="G74" s="4" t="inlineStr">
+        <is>
+          <t>01:13:55</t>
+        </is>
+      </c>
+      <c r="H74" s="4" t="n">
+        <v>3.111</v>
+      </c>
+      <c r="I74" s="4" t="n">
+        <v>1.282250586486312</v>
+      </c>
+      <c r="J74" s="4" t="inlineStr">
+        <is>
+          <t>EX-2025-73252434-   -APN-SDYME#ENACOM</t>
+        </is>
+      </c>
+      <c r="K74" s="4" t="inlineStr">
+        <is>
+          <t>EF0391</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="4" t="inlineStr">
+        <is>
+          <t>Posadas</t>
+        </is>
+      </c>
+      <c r="B75" s="4" t="inlineStr">
+        <is>
+          <t>Formosa</t>
+        </is>
+      </c>
+      <c r="C75" s="4" t="inlineStr">
+        <is>
+          <t>Formosa</t>
+        </is>
+      </c>
+      <c r="D75" s="5" t="n">
+        <v>45847.47630787037</v>
+      </c>
+      <c r="E75" s="5" t="n">
+        <v>45848.71959490741</v>
+      </c>
+      <c r="F75" s="4" t="n">
+        <v>5553</v>
+      </c>
+      <c r="G75" s="4" t="inlineStr">
+        <is>
+          <t>10:32:42</t>
+        </is>
+      </c>
+      <c r="H75" s="4" t="n">
+        <v>8.835000000000001</v>
+      </c>
+      <c r="I75" s="4" t="n">
+        <v>10.34155847235734</v>
+      </c>
+      <c r="J75" s="4" t="inlineStr">
+        <is>
+          <t>EX-2025-77142320-   -APN-SDYME#ENACOM</t>
+        </is>
+      </c>
+      <c r="K75" s="4" t="inlineStr">
+        <is>
+          <t>EF0391</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="4" t="inlineStr">
+        <is>
+          <t>Posadas</t>
+        </is>
+      </c>
+      <c r="B76" s="4" t="inlineStr">
+        <is>
+          <t>Formosa</t>
+        </is>
+      </c>
+      <c r="C76" s="4" t="inlineStr">
+        <is>
+          <t>Laguna Blanca</t>
+        </is>
+      </c>
+      <c r="D76" s="5" t="n">
+        <v>45846.4572337963</v>
+      </c>
+      <c r="E76" s="5" t="n">
+        <v>45846.50842592592</v>
+      </c>
+      <c r="F76" s="4" t="n">
+        <v>610</v>
+      </c>
+      <c r="G76" s="4" t="inlineStr">
+        <is>
+          <t>01:13:43</t>
+        </is>
+      </c>
+      <c r="H76" s="4" t="n">
+        <v>2.874</v>
+      </c>
+      <c r="I76" s="4" t="n">
+        <v>1.094325229066509</v>
+      </c>
+      <c r="J76" s="4" t="inlineStr">
+        <is>
+          <t>EX-2025-77142546-   -APN-SDYME#ENACOM</t>
+        </is>
+      </c>
+      <c r="K76" s="4" t="inlineStr">
+        <is>
+          <t>EF0391</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="4" t="inlineStr">
+        <is>
           <t>Salta</t>
         </is>
       </c>
-      <c r="B67" s="4" t="inlineStr">
+      <c r="B77" s="4" t="inlineStr">
+        <is>
+          <t>Catamarca</t>
+        </is>
+      </c>
+      <c r="C77" s="4" t="inlineStr">
+        <is>
+          <t>San Fernando del Valle de Catamarca</t>
+        </is>
+      </c>
+      <c r="D77" s="5" t="n">
+        <v>45910.42053240741</v>
+      </c>
+      <c r="E77" s="5" t="n">
+        <v>45911.89583333334</v>
+      </c>
+      <c r="F77" s="4" t="n">
+        <v>7768</v>
+      </c>
+      <c r="G77" s="4" t="inlineStr">
+        <is>
+          <t>17:24:07</t>
+        </is>
+      </c>
+      <c r="H77" s="4" t="n">
+        <v>9.185</v>
+      </c>
+      <c r="I77" s="4" t="n">
+        <v>11.17715324638573</v>
+      </c>
+      <c r="J77" s="4" t="inlineStr">
+        <is>
+          <t>COMPLETAR</t>
+        </is>
+      </c>
+      <c r="K77" s="4" t="inlineStr">
+        <is>
+          <t>EF1891</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="4" t="inlineStr">
+        <is>
+          <t>Salta</t>
+        </is>
+      </c>
+      <c r="B78" s="4" t="inlineStr">
         <is>
           <t>Jujuy</t>
         </is>
       </c>
-      <c r="C67" s="4" t="inlineStr">
+      <c r="C78" s="4" t="inlineStr">
+        <is>
+          <t>San Pablo de Reyes</t>
+        </is>
+      </c>
+      <c r="D78" s="5" t="n">
+        <v>45734.39631944444</v>
+      </c>
+      <c r="E78" s="5" t="n">
+        <v>45734.41811342593</v>
+      </c>
+      <c r="F78" s="4" t="n">
+        <v>260</v>
+      </c>
+      <c r="G78" s="4" t="inlineStr">
+        <is>
+          <t>00:25:35</t>
+        </is>
+      </c>
+      <c r="H78" s="4" t="n">
+        <v>4.246</v>
+      </c>
+      <c r="I78" s="4" t="n">
+        <v>2.388541898380706</v>
+      </c>
+      <c r="J78" s="4" t="inlineStr">
+        <is>
+          <t>EX-2025-33150525-   -APN-SDYME#ENACOM</t>
+        </is>
+      </c>
+      <c r="K78" s="4" t="inlineStr">
+        <is>
+          <t>EF1891</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="4" t="inlineStr">
+        <is>
+          <t>Salta</t>
+        </is>
+      </c>
+      <c r="B79" s="4" t="inlineStr">
+        <is>
+          <t>Jujuy</t>
+        </is>
+      </c>
+      <c r="C79" s="4" t="inlineStr">
+        <is>
+          <t>San Salvador de Jujuy</t>
+        </is>
+      </c>
+      <c r="D79" s="5" t="n">
+        <v>45734.45050925926</v>
+      </c>
+      <c r="E79" s="5" t="n">
+        <v>45736.80579861111</v>
+      </c>
+      <c r="F79" s="4" t="n">
+        <v>7808</v>
+      </c>
+      <c r="G79" s="4" t="inlineStr">
+        <is>
+          <t>17:51:37</t>
+        </is>
+      </c>
+      <c r="H79" s="4" t="n">
+        <v>16.837</v>
+      </c>
+      <c r="I79" s="4" t="n">
+        <v>37.55798705788629</v>
+      </c>
+      <c r="J79" s="4" t="inlineStr">
+        <is>
+          <t>EX-2025-101525989- -APN-SDYME#ENACOM</t>
+        </is>
+      </c>
+      <c r="K79" s="4" t="inlineStr">
+        <is>
+          <t>EF0391, EF1891</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="4" t="inlineStr">
+        <is>
+          <t>Salta</t>
+        </is>
+      </c>
+      <c r="B80" s="4" t="inlineStr">
+        <is>
+          <t>Jujuy</t>
+        </is>
+      </c>
+      <c r="C80" s="4" t="inlineStr">
         <is>
           <t>Villa Jardín de Reyes</t>
         </is>
       </c>
-      <c r="D67" s="5" t="n">
+      <c r="D80" s="5" t="n">
         <v>45733.61721064815</v>
       </c>
-      <c r="E67" s="5" t="n">
+      <c r="E80" s="5" t="n">
         <v>45733.67739583334</v>
       </c>
-      <c r="F67" s="4" t="n">
+      <c r="F80" s="4" t="n">
         <v>545</v>
       </c>
-      <c r="G67" s="4" t="inlineStr">
+      <c r="G80" s="4" t="inlineStr">
         <is>
           <t>01:26:40</t>
         </is>
       </c>
-      <c r="H67" s="4" t="n">
+      <c r="H80" s="4" t="n">
         <v>2.843</v>
       </c>
-      <c r="I67" s="4" t="n">
+      <c r="I80" s="4" t="n">
         <v>1.070844976170247</v>
       </c>
-      <c r="J67" s="4" t="inlineStr">
+      <c r="J80" s="4" t="inlineStr">
         <is>
           <t>EX-2025-33162392-   -APN-SDYME#ENACOM</t>
         </is>
       </c>
-      <c r="K67" s="4" t="inlineStr">
+      <c r="K80" s="4" t="inlineStr">
         <is>
           <t>EF1891</t>
         </is>

</xml_diff>